<commit_message>
Se obtienen resultados para concrete06
</commit_message>
<xml_diff>
--- a/Validacion/RW-A20-P10-S38/Documentation/Documentacion RW-A20-P10-S38.xlsx
+++ b/Validacion/RW-A20-P10-S38/Documentation/Documentacion RW-A20-P10-S38.xlsx
@@ -2723,6 +2723,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2735,41 +2744,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11708,12 +11708,12 @@
       <c r="V8" s="75"/>
     </row>
     <row r="9" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D9" s="262" t="s">
+      <c r="D9" s="257" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="263"/>
-      <c r="F9" s="263"/>
-      <c r="G9" s="264"/>
+      <c r="E9" s="258"/>
+      <c r="F9" s="258"/>
+      <c r="G9" s="259"/>
       <c r="V9" s="75"/>
     </row>
     <row r="10" spans="4:23" x14ac:dyDescent="0.25">
@@ -12059,7 +12059,7 @@
       <c r="D31" s="96"/>
     </row>
     <row r="32" spans="3:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="265" t="s">
+      <c r="C32" s="264" t="s">
         <v>207</v>
       </c>
       <c r="D32" s="85" t="s">
@@ -12070,7 +12070,7 @@
       <c r="G32" s="87"/>
     </row>
     <row r="33" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C33" s="266"/>
+      <c r="C33" s="265"/>
       <c r="D33" s="89" t="s">
         <v>180</v>
       </c>
@@ -12081,7 +12081,7 @@
       <c r="G33" s="87"/>
     </row>
     <row r="34" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C34" s="266"/>
+      <c r="C34" s="265"/>
       <c r="D34" s="90" t="s">
         <v>181</v>
       </c>
@@ -12091,7 +12091,7 @@
       <c r="G34" s="88"/>
     </row>
     <row r="35" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C35" s="266"/>
+      <c r="C35" s="265"/>
       <c r="D35" s="90" t="s">
         <v>183</v>
       </c>
@@ -12103,7 +12103,7 @@
       </c>
     </row>
     <row r="36" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C36" s="266"/>
+      <c r="C36" s="265"/>
       <c r="D36" s="91" t="s">
         <v>185</v>
       </c>
@@ -12118,7 +12118,7 @@
       </c>
     </row>
     <row r="37" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C37" s="266"/>
+      <c r="C37" s="265"/>
       <c r="D37" s="94" t="s">
         <v>187</v>
       </c>
@@ -12131,7 +12131,7 @@
       </c>
     </row>
     <row r="38" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C38" s="266"/>
+      <c r="C38" s="265"/>
       <c r="D38" s="89" t="s">
         <v>193</v>
       </c>
@@ -12156,7 +12156,7 @@
       </c>
     </row>
     <row r="39" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C39" s="266"/>
+      <c r="C39" s="265"/>
       <c r="D39" s="90" t="s">
         <v>194</v>
       </c>
@@ -12178,7 +12178,7 @@
       </c>
     </row>
     <row r="40" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C40" s="266"/>
+      <c r="C40" s="265"/>
       <c r="D40" s="90" t="s">
         <v>195</v>
       </c>
@@ -12219,7 +12219,7 @@
       </c>
     </row>
     <row r="41" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C41" s="266"/>
+      <c r="C41" s="265"/>
       <c r="D41" s="91" t="s">
         <v>196</v>
       </c>
@@ -12260,7 +12260,7 @@
       </c>
     </row>
     <row r="42" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C42" s="266"/>
+      <c r="C42" s="265"/>
       <c r="D42" s="80" t="s">
         <v>197</v>
       </c>
@@ -12293,15 +12293,15 @@
       </c>
     </row>
     <row r="43" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C43" s="266"/>
+      <c r="C43" s="265"/>
       <c r="D43" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E43" s="257" t="s">
+      <c r="E43" s="260" t="s">
         <v>200</v>
       </c>
-      <c r="F43" s="257"/>
-      <c r="G43" s="258"/>
+      <c r="F43" s="260"/>
+      <c r="G43" s="261"/>
       <c r="AA43" s="44">
         <v>13</v>
       </c>
@@ -12330,13 +12330,13 @@
       </c>
     </row>
     <row r="44" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C44" s="267"/>
+      <c r="C44" s="266"/>
       <c r="D44" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="E44" s="259"/>
-      <c r="F44" s="259"/>
-      <c r="G44" s="260"/>
+      <c r="E44" s="262"/>
+      <c r="F44" s="262"/>
+      <c r="G44" s="263"/>
       <c r="AA44" s="44">
         <v>14</v>
       </c>
@@ -12365,7 +12365,7 @@
       </c>
     </row>
     <row r="45" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C45" s="261" t="s">
+      <c r="C45" s="272" t="s">
         <v>216</v>
       </c>
       <c r="D45" s="94" t="s">
@@ -12402,7 +12402,7 @@
       </c>
     </row>
     <row r="46" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C46" s="261"/>
+      <c r="C46" s="272"/>
       <c r="D46" s="89" t="s">
         <v>180</v>
       </c>
@@ -12439,7 +12439,7 @@
       </c>
     </row>
     <row r="47" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C47" s="261"/>
+      <c r="C47" s="272"/>
       <c r="D47" s="90" t="s">
         <v>181</v>
       </c>
@@ -12475,7 +12475,7 @@
       </c>
     </row>
     <row r="48" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C48" s="261"/>
+      <c r="C48" s="272"/>
       <c r="D48" s="90" t="s">
         <v>183</v>
       </c>
@@ -12513,7 +12513,7 @@
       </c>
     </row>
     <row r="49" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C49" s="261"/>
+      <c r="C49" s="272"/>
       <c r="D49" s="90" t="s">
         <v>185</v>
       </c>
@@ -12554,7 +12554,7 @@
       </c>
     </row>
     <row r="50" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C50" s="261"/>
+      <c r="C50" s="272"/>
       <c r="D50" s="93" t="s">
         <v>187</v>
       </c>
@@ -12587,7 +12587,7 @@
       </c>
     </row>
     <row r="51" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C51" s="261"/>
+      <c r="C51" s="272"/>
       <c r="D51" s="90" t="s">
         <v>212</v>
       </c>
@@ -12628,7 +12628,7 @@
       </c>
     </row>
     <row r="52" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C52" s="261"/>
+      <c r="C52" s="272"/>
       <c r="D52" s="93" t="s">
         <v>197</v>
       </c>
@@ -12661,15 +12661,15 @@
       </c>
     </row>
     <row r="53" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C53" s="261"/>
+      <c r="C53" s="272"/>
       <c r="D53" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="257" t="s">
+      <c r="E53" s="260" t="s">
         <v>200</v>
       </c>
-      <c r="F53" s="257"/>
-      <c r="G53" s="258"/>
+      <c r="F53" s="260"/>
+      <c r="G53" s="261"/>
       <c r="AA53" s="44">
         <v>23</v>
       </c>
@@ -12698,13 +12698,13 @@
       </c>
     </row>
     <row r="54" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C54" s="261"/>
+      <c r="C54" s="272"/>
       <c r="D54" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E54" s="259"/>
-      <c r="F54" s="259"/>
-      <c r="G54" s="260"/>
+      <c r="E54" s="262"/>
+      <c r="F54" s="262"/>
+      <c r="G54" s="263"/>
       <c r="AA54" s="44">
         <v>24</v>
       </c>
@@ -12733,7 +12733,7 @@
       </c>
     </row>
     <row r="55" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C55" s="261"/>
+      <c r="C55" s="272"/>
       <c r="D55" s="94" t="s">
         <v>186</v>
       </c>
@@ -12768,7 +12768,7 @@
       </c>
     </row>
     <row r="56" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C56" s="261"/>
+      <c r="C56" s="272"/>
       <c r="D56" s="89" t="s">
         <v>180</v>
       </c>
@@ -12805,7 +12805,7 @@
       </c>
     </row>
     <row r="57" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C57" s="261"/>
+      <c r="C57" s="272"/>
       <c r="D57" s="90" t="s">
         <v>181</v>
       </c>
@@ -12841,7 +12841,7 @@
       </c>
     </row>
     <row r="58" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C58" s="261"/>
+      <c r="C58" s="272"/>
       <c r="D58" s="90" t="s">
         <v>183</v>
       </c>
@@ -12879,7 +12879,7 @@
       </c>
     </row>
     <row r="59" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C59" s="261"/>
+      <c r="C59" s="272"/>
       <c r="D59" s="91" t="s">
         <v>185</v>
       </c>
@@ -12920,7 +12920,7 @@
       </c>
     </row>
     <row r="60" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C60" s="261"/>
+      <c r="C60" s="272"/>
       <c r="D60" s="94" t="s">
         <v>187</v>
       </c>
@@ -12955,7 +12955,7 @@
       </c>
     </row>
     <row r="61" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C61" s="261"/>
+      <c r="C61" s="272"/>
       <c r="D61" s="89" t="s">
         <v>212</v>
       </c>
@@ -12996,7 +12996,7 @@
       </c>
     </row>
     <row r="62" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C62" s="261"/>
+      <c r="C62" s="272"/>
       <c r="D62" s="93" t="s">
         <v>197</v>
       </c>
@@ -13029,15 +13029,15 @@
       </c>
     </row>
     <row r="63" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C63" s="261"/>
+      <c r="C63" s="272"/>
       <c r="D63" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E63" s="257" t="s">
+      <c r="E63" s="260" t="s">
         <v>200</v>
       </c>
-      <c r="F63" s="257"/>
-      <c r="G63" s="258"/>
+      <c r="F63" s="260"/>
+      <c r="G63" s="261"/>
       <c r="AA63" s="44">
         <v>33</v>
       </c>
@@ -13066,13 +13066,13 @@
       </c>
     </row>
     <row r="64" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C64" s="261"/>
+      <c r="C64" s="272"/>
       <c r="D64" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="259"/>
-      <c r="F64" s="259"/>
-      <c r="G64" s="260"/>
+      <c r="E64" s="262"/>
+      <c r="F64" s="262"/>
+      <c r="G64" s="263"/>
       <c r="AA64" s="44">
         <v>34</v>
       </c>
@@ -13224,22 +13224,22 @@
       </c>
     </row>
     <row r="69" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C69" s="265" t="s">
+      <c r="C69" s="264" t="s">
         <v>160</v>
       </c>
-      <c r="D69" s="271" t="s">
+      <c r="D69" s="270" t="s">
         <v>161</v>
       </c>
-      <c r="E69" s="271"/>
-      <c r="F69" s="271" t="s">
+      <c r="E69" s="270"/>
+      <c r="F69" s="270" t="s">
         <v>133</v>
       </c>
-      <c r="G69" s="272"/>
-      <c r="I69" s="268" t="s">
+      <c r="G69" s="271"/>
+      <c r="I69" s="267" t="s">
         <v>223</v>
       </c>
-      <c r="J69" s="269"/>
-      <c r="K69" s="270"/>
+      <c r="J69" s="268"/>
+      <c r="K69" s="269"/>
       <c r="AA69" s="44">
         <v>39</v>
       </c>
@@ -13268,7 +13268,7 @@
       </c>
     </row>
     <row r="70" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C70" s="266"/>
+      <c r="C70" s="265"/>
       <c r="D70" s="15" t="s">
         <v>162</v>
       </c>
@@ -13676,11 +13676,11 @@
         <f t="shared" si="10"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="I77" s="268" t="s">
+      <c r="I77" s="267" t="s">
         <v>222</v>
       </c>
-      <c r="J77" s="269"/>
-      <c r="K77" s="270"/>
+      <c r="J77" s="268"/>
+      <c r="K77" s="269"/>
       <c r="AA77" s="44">
         <v>47</v>
       </c>
@@ -15510,12 +15510,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="E53:G54"/>
+    <mergeCell ref="E63:G64"/>
+    <mergeCell ref="C45:C64"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="E43:G44"/>
@@ -15525,12 +15525,12 @@
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="F69:G69"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="E53:G54"/>
-    <mergeCell ref="E63:G64"/>
-    <mergeCell ref="C45:C64"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="C130:C131"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15580,27 +15580,27 @@
       <c r="L4" s="81"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="268" t="s">
+      <c r="C5" s="267" t="s">
         <v>314</v>
       </c>
-      <c r="D5" s="269"/>
-      <c r="E5" s="269"/>
-      <c r="F5" s="269"/>
-      <c r="G5" s="269"/>
-      <c r="H5" s="270"/>
+      <c r="D5" s="268"/>
+      <c r="E5" s="268"/>
+      <c r="F5" s="268"/>
+      <c r="G5" s="268"/>
+      <c r="H5" s="269"/>
       <c r="I5" s="171" t="s">
         <v>315</v>
       </c>
-      <c r="J5" s="268" t="s">
+      <c r="J5" s="267" t="s">
         <v>316</v>
       </c>
-      <c r="K5" s="269"/>
-      <c r="L5" s="269"/>
+      <c r="K5" s="268"/>
+      <c r="L5" s="268"/>
       <c r="M5" s="273" t="s">
         <v>322</v>
       </c>
-      <c r="N5" s="271"/>
-      <c r="O5" s="272"/>
+      <c r="N5" s="270"/>
+      <c r="O5" s="271"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="168" t="s">
@@ -16294,7 +16294,7 @@
   <dimension ref="B2:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16319,7 +16319,7 @@
         <v>359</v>
       </c>
       <c r="C3" s="207">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -16349,11 +16349,11 @@
       </c>
       <c r="D6" s="224">
         <f>C6/$C$3</f>
-        <v>12.192</v>
+        <v>24.384</v>
       </c>
       <c r="E6" s="224">
         <f>INT(D6)</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F6" s="225">
         <f>E6*$C$3</f>
@@ -16361,7 +16361,7 @@
       </c>
       <c r="G6">
         <f>E6*4*3</f>
-        <v>144</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -16374,19 +16374,19 @@
       </c>
       <c r="D7" s="224">
         <f t="shared" ref="D7:D13" si="1">C7/$C$3</f>
-        <v>36.576000000000001</v>
+        <v>73.152000000000001</v>
       </c>
       <c r="E7" s="224">
         <f t="shared" ref="E7:E13" si="2">INT(D7)</f>
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="F7" s="225">
         <f t="shared" ref="F7:F13" si="3">E7*$C$3</f>
-        <v>7.2</v>
+        <v>7.3000000000000007</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G13" si="4">E7*4*3</f>
-        <v>432</v>
+        <f t="shared" ref="G7:G11" si="4">E7*4*3</f>
+        <v>876</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -16399,19 +16399,19 @@
       </c>
       <c r="D8" s="224">
         <f t="shared" si="1"/>
-        <v>60.96</v>
+        <v>121.92</v>
       </c>
       <c r="E8" s="224">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="F8" s="225">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>12.100000000000001</v>
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>720</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -16424,11 +16424,11 @@
       </c>
       <c r="D9" s="224">
         <f t="shared" si="1"/>
-        <v>85.343999999999994</v>
+        <v>170.68799999999999</v>
       </c>
       <c r="E9" s="224">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="F9" s="225">
         <f t="shared" si="3"/>
@@ -16436,7 +16436,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>1020</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -16449,19 +16449,19 @@
       </c>
       <c r="D10" s="224">
         <f t="shared" si="1"/>
-        <v>121.92</v>
+        <v>243.84</v>
       </c>
       <c r="E10" s="224">
         <f t="shared" si="2"/>
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="F10" s="225">
         <f t="shared" si="3"/>
-        <v>24.200000000000003</v>
+        <v>24.3</v>
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>1452</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -16474,19 +16474,19 @@
       </c>
       <c r="D11" s="224">
         <f t="shared" si="1"/>
-        <v>182.88</v>
+        <v>365.76</v>
       </c>
       <c r="E11" s="224">
         <f t="shared" si="2"/>
-        <v>182</v>
+        <v>365</v>
       </c>
       <c r="F11" s="225">
         <f t="shared" si="3"/>
-        <v>36.4</v>
+        <v>36.5</v>
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>2184</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -16499,11 +16499,11 @@
       </c>
       <c r="D12" s="224">
         <f t="shared" si="1"/>
-        <v>268.22399999999999</v>
+        <v>536.44799999999998</v>
       </c>
       <c r="E12" s="224">
         <f t="shared" si="2"/>
-        <v>268</v>
+        <v>536</v>
       </c>
       <c r="F12" s="225">
         <f t="shared" si="3"/>
@@ -16511,7 +16511,7 @@
       </c>
       <c r="G12">
         <f>E12*4*2</f>
-        <v>2144</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -16524,33 +16524,33 @@
       </c>
       <c r="D13" s="227">
         <f t="shared" si="1"/>
-        <v>377.952</v>
+        <v>755.904</v>
       </c>
       <c r="E13" s="227">
         <f t="shared" si="2"/>
-        <v>377</v>
+        <v>755</v>
       </c>
       <c r="F13" s="230">
         <f t="shared" si="3"/>
-        <v>75.400000000000006</v>
+        <v>75.5</v>
       </c>
       <c r="G13">
         <f>E13*4*2</f>
-        <v>3016</v>
+        <v>6040</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D14" s="228">
         <f>SUM(D6:D13)*4</f>
-        <v>4584.192</v>
+        <v>9168.384</v>
       </c>
       <c r="E14" s="228">
         <f>SUM(E6:E13)*4</f>
-        <v>4564</v>
+        <v>9148</v>
       </c>
       <c r="G14">
         <f>SUM(G6:G13)</f>
-        <v>11112</v>
+        <v>22280</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -16591,11 +16591,11 @@
       </c>
       <c r="D19" s="224">
         <f>C19/$C$3</f>
-        <v>34.137599999999999</v>
+        <v>68.275199999999998</v>
       </c>
       <c r="E19" s="224">
         <f>INT(D19)</f>
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="F19" s="225">
         <f>E19*$C$3</f>
@@ -16612,11 +16612,11 @@
       </c>
       <c r="D20" s="224">
         <f t="shared" ref="D20:D26" si="6">C20/$C$3</f>
-        <v>46.329600000000006</v>
+        <v>92.659200000000013</v>
       </c>
       <c r="E20" s="224">
         <f t="shared" ref="E20:E26" si="7">INT(D20)</f>
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="F20" s="225">
         <f t="shared" ref="F20:F26" si="8">E20*$C$3</f>
@@ -16633,11 +16633,11 @@
       </c>
       <c r="D21" s="224">
         <f t="shared" si="6"/>
-        <v>68.275199999999998</v>
+        <v>136.5504</v>
       </c>
       <c r="E21" s="224">
         <f t="shared" si="7"/>
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F21" s="225">
         <f t="shared" si="8"/>
@@ -16654,11 +16654,11 @@
       </c>
       <c r="D22" s="224">
         <f t="shared" si="6"/>
-        <v>91.44</v>
+        <v>182.88</v>
       </c>
       <c r="E22" s="224">
         <f t="shared" si="7"/>
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="F22" s="225">
         <f t="shared" si="8"/>
@@ -16675,11 +16675,11 @@
       </c>
       <c r="D23" s="224">
         <f t="shared" si="6"/>
-        <v>134.11199999999999</v>
+        <v>268.22399999999999</v>
       </c>
       <c r="E23" s="224">
         <f t="shared" si="7"/>
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="F23" s="225">
         <f t="shared" si="8"/>
@@ -16696,15 +16696,15 @@
       </c>
       <c r="D24" s="224">
         <f t="shared" si="6"/>
-        <v>182.88</v>
+        <v>365.76</v>
       </c>
       <c r="E24" s="224">
         <f t="shared" si="7"/>
-        <v>182</v>
+        <v>365</v>
       </c>
       <c r="F24" s="225">
         <f t="shared" si="8"/>
-        <v>36.4</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -16717,11 +16717,11 @@
       </c>
       <c r="D25" s="224">
         <f t="shared" si="6"/>
-        <v>280.416</v>
+        <v>560.83199999999999</v>
       </c>
       <c r="E25" s="224">
         <f t="shared" si="7"/>
-        <v>280</v>
+        <v>560</v>
       </c>
       <c r="F25" s="225">
         <f t="shared" si="8"/>
@@ -16738,25 +16738,25 @@
       </c>
       <c r="D26" s="227">
         <f t="shared" si="6"/>
-        <v>377.952</v>
+        <v>755.904</v>
       </c>
       <c r="E26" s="227">
         <f t="shared" si="7"/>
-        <v>377</v>
+        <v>755</v>
       </c>
       <c r="F26" s="230">
         <f t="shared" si="8"/>
-        <v>75.400000000000006</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D27" s="228">
         <f>SUM(D19:D26)*4</f>
-        <v>4862.1696000000002</v>
+        <v>9724.3392000000003</v>
       </c>
       <c r="E27" s="228">
         <f>SUM(E19:E26)*4</f>
-        <v>4848</v>
+        <v>9704</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se modifican parametros fcu y ecu de hormigon para ejemplo RW-A20-P10-S38
</commit_message>
<xml_diff>
--- a/Validacion/RW-A20-P10-S38/Documentation/Documentacion RW-A20-P10-S38.xlsx
+++ b/Validacion/RW-A20-P10-S38/Documentation/Documentacion RW-A20-P10-S38.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryj\Documents\GitHub\Ejemplos\Validacion\RW-A20-P10-S38\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B604D5E1-A58E-48BB-94E2-9CF21E8E241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4E4A7E-46FD-4EFB-A3D4-74478D5D3DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prop Geom y de Materiales" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="380">
   <si>
     <t>m</t>
   </si>
@@ -1449,6 +1449,36 @@
   </si>
   <si>
     <t>Load Step fin drift</t>
+  </si>
+  <si>
+    <t>Gfc</t>
+  </si>
+  <si>
+    <t>N/mm</t>
+  </si>
+  <si>
+    <t>ec</t>
+  </si>
+  <si>
+    <t>Lelem</t>
+  </si>
+  <si>
+    <t>er</t>
+  </si>
+  <si>
+    <t>Ec</t>
+  </si>
+  <si>
+    <t>No confinado</t>
+  </si>
+  <si>
+    <t>Confinado</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -2144,7 +2174,7 @@
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2655,6 +2685,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2730,6 +2766,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2739,18 +2790,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2775,9 +2814,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2802,12 +2838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -7190,16 +7221,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>355502</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520651</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>398145</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>95736</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>288245</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>150981</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7222,8 +7253,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="355502" y="1466850"/>
-          <a:ext cx="4319368" cy="4282926"/>
+          <a:off x="4787851" y="5000625"/>
+          <a:ext cx="3971929" cy="4608681"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>372828</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>250600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>60048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74B8AF20-348F-D69C-EB9B-29E42EE42F7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13517328" y="4819650"/>
+          <a:ext cx="4417387" cy="4694913"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7904,20 +7979,20 @@
   <sheetData>
     <row r="1" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="235" t="s">
+      <c r="J2" s="237" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="236"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="236"/>
-      <c r="N2" s="237"/>
-      <c r="Q2" s="235" t="s">
+      <c r="K2" s="238"/>
+      <c r="L2" s="238"/>
+      <c r="M2" s="238"/>
+      <c r="N2" s="239"/>
+      <c r="Q2" s="237" t="s">
         <v>336</v>
       </c>
-      <c r="R2" s="236"/>
-      <c r="S2" s="236"/>
-      <c r="T2" s="236"/>
-      <c r="U2" s="237"/>
+      <c r="R2" s="238"/>
+      <c r="S2" s="238"/>
+      <c r="T2" s="238"/>
+      <c r="U2" s="239"/>
     </row>
     <row r="3" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J3" s="11"/>
@@ -7929,7 +8004,7 @@
       <c r="N3" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="Q3" s="241" t="s">
+      <c r="Q3" s="243" t="s">
         <v>3</v>
       </c>
       <c r="R3" s="18" t="s">
@@ -7956,7 +8031,7 @@
         <f>M4/25.4</f>
         <v>96.000000000000014</v>
       </c>
-      <c r="Q4" s="242"/>
+      <c r="Q4" s="244"/>
       <c r="R4" s="1"/>
       <c r="S4" s="166"/>
       <c r="T4" s="2"/>
@@ -7976,7 +8051,7 @@
         <f>M5/25.4</f>
         <v>48.031496062992126</v>
       </c>
-      <c r="Q5" s="242"/>
+      <c r="Q5" s="244"/>
       <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
@@ -7998,7 +8073,7 @@
         <f t="shared" ref="N6:N7" si="0">M6/25.4</f>
         <v>6.0000000000000009</v>
       </c>
-      <c r="Q6" s="242"/>
+      <c r="Q6" s="244"/>
       <c r="R6" s="23" t="s">
         <v>6</v>
       </c>
@@ -8020,7 +8095,7 @@
         <f t="shared" si="0"/>
         <v>12.000000000000002</v>
       </c>
-      <c r="Q7" s="242"/>
+      <c r="Q7" s="244"/>
       <c r="R7" s="23" t="s">
         <v>7</v>
       </c>
@@ -8049,7 +8124,7 @@
         <f>M8/25.4</f>
         <v>9</v>
       </c>
-      <c r="Q8" s="242"/>
+      <c r="Q8" s="244"/>
       <c r="R8" s="23" t="s">
         <v>10</v>
       </c>
@@ -8074,7 +8149,7 @@
       <c r="N9" s="200" t="s">
         <v>353</v>
       </c>
-      <c r="Q9" s="242"/>
+      <c r="Q9" s="244"/>
       <c r="R9" s="3" t="s">
         <v>11</v>
       </c>
@@ -8087,7 +8162,7 @@
       <c r="U9" s="29"/>
     </row>
     <row r="10" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q10" s="242"/>
+      <c r="Q10" s="244"/>
       <c r="R10" s="6" t="s">
         <v>13</v>
       </c>
@@ -8096,14 +8171,14 @@
       <c r="U10" s="30"/>
     </row>
     <row r="11" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="238" t="s">
+      <c r="J11" s="240" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="239"/>
-      <c r="L11" s="239"/>
-      <c r="M11" s="239"/>
-      <c r="N11" s="240"/>
-      <c r="Q11" s="242"/>
+      <c r="K11" s="241"/>
+      <c r="L11" s="241"/>
+      <c r="M11" s="241"/>
+      <c r="N11" s="242"/>
+      <c r="Q11" s="244"/>
       <c r="R11" s="23" t="s">
         <v>6</v>
       </c>
@@ -8127,7 +8202,7 @@
       <c r="N12" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="Q12" s="242"/>
+      <c r="Q12" s="244"/>
       <c r="R12" s="23" t="s">
         <v>7</v>
       </c>
@@ -8159,7 +8234,7 @@
         <f>M13/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="242"/>
+      <c r="Q13" s="244"/>
       <c r="R13" s="23" t="s">
         <v>10</v>
       </c>
@@ -8187,7 +8262,7 @@
         <f t="shared" ref="N14:N32" si="2">M14/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="242"/>
+      <c r="Q14" s="244"/>
       <c r="R14" s="3" t="s">
         <v>11</v>
       </c>
@@ -8221,7 +8296,7 @@
         <f>M15-$M$15/2</f>
         <v>157.845</v>
       </c>
-      <c r="Q15" s="242"/>
+      <c r="Q15" s="244"/>
       <c r="R15" s="6" t="s">
         <v>16</v>
       </c>
@@ -8251,7 +8326,7 @@
         <f t="shared" ref="O16:O26" si="3">M16-$M$15/2</f>
         <v>157.845</v>
       </c>
-      <c r="Q16" s="242"/>
+      <c r="Q16" s="244"/>
       <c r="R16" s="23" t="s">
         <v>6</v>
       </c>
@@ -8281,7 +8356,7 @@
         <f>M17-$M$15/2</f>
         <v>473.52499999999998</v>
       </c>
-      <c r="Q17" s="242"/>
+      <c r="Q17" s="244"/>
       <c r="R17" s="23" t="s">
         <v>7</v>
       </c>
@@ -8317,7 +8392,7 @@
         <f t="shared" si="3"/>
         <v>473.52499999999998</v>
       </c>
-      <c r="Q18" s="242"/>
+      <c r="Q18" s="244"/>
       <c r="R18" s="23" t="s">
         <v>10</v>
       </c>
@@ -8349,7 +8424,7 @@
         <f t="shared" si="3"/>
         <v>789.21499999999992</v>
       </c>
-      <c r="Q19" s="242"/>
+      <c r="Q19" s="244"/>
       <c r="R19" s="3" t="s">
         <v>11</v>
       </c>
@@ -8384,7 +8459,7 @@
         <f t="shared" si="3"/>
         <v>789.21499999999992</v>
       </c>
-      <c r="Q20" s="242"/>
+      <c r="Q20" s="244"/>
       <c r="R20" s="32" t="s">
         <v>19</v>
       </c>
@@ -8420,7 +8495,7 @@
         <f t="shared" si="3"/>
         <v>1104.895</v>
       </c>
-      <c r="Q21" s="242"/>
+      <c r="Q21" s="244"/>
       <c r="R21" s="32" t="s">
         <v>21</v>
       </c>
@@ -8454,7 +8529,7 @@
         <f t="shared" si="3"/>
         <v>1104.895</v>
       </c>
-      <c r="Q22" s="242"/>
+      <c r="Q22" s="244"/>
       <c r="R22" s="32" t="s">
         <v>24</v>
       </c>
@@ -8488,7 +8563,7 @@
         <f t="shared" si="3"/>
         <v>1420.585</v>
       </c>
-      <c r="Q23" s="243"/>
+      <c r="Q23" s="245"/>
       <c r="R23" s="2"/>
       <c r="S23" s="8" t="s">
         <v>26</v>
@@ -8520,7 +8595,7 @@
         <f t="shared" si="3"/>
         <v>1420.585</v>
       </c>
-      <c r="Q24" s="244" t="s">
+      <c r="Q24" s="246" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -8554,7 +8629,7 @@
         <f t="shared" si="3"/>
         <v>1736.2649999999999</v>
       </c>
-      <c r="Q25" s="242"/>
+      <c r="Q25" s="244"/>
       <c r="R25" s="6" t="s">
         <v>29</v>
       </c>
@@ -8584,7 +8659,7 @@
         <f t="shared" si="3"/>
         <v>1736.2649999999999</v>
       </c>
-      <c r="Q26" s="242"/>
+      <c r="Q26" s="244"/>
       <c r="R26" s="23" t="s">
         <v>30</v>
       </c>
@@ -8620,7 +8695,7 @@
         <f>M27-$M$15/2</f>
         <v>2051.9550000000004</v>
       </c>
-      <c r="Q27" s="242"/>
+      <c r="Q27" s="244"/>
       <c r="R27" s="23" t="s">
         <v>32</v>
       </c>
@@ -8654,7 +8729,7 @@
         <f>M28-$M$15/2</f>
         <v>2051.9550000000004</v>
       </c>
-      <c r="Q28" s="242"/>
+      <c r="Q28" s="244"/>
       <c r="R28" s="23" t="s">
         <v>19</v>
       </c>
@@ -8691,7 +8766,7 @@
         <f>M29-228.6/2</f>
         <v>2324.1</v>
       </c>
-      <c r="Q29" s="242"/>
+      <c r="Q29" s="244"/>
       <c r="R29" s="23" t="s">
         <v>34</v>
       </c>
@@ -8723,7 +8798,7 @@
         <v>96.000000000000014</v>
       </c>
       <c r="O30" s="178"/>
-      <c r="Q30" s="242"/>
+      <c r="Q30" s="244"/>
       <c r="R30" s="23" t="s">
         <v>36</v>
       </c>
@@ -8755,7 +8830,7 @@
         <v>105</v>
       </c>
       <c r="O31" s="178"/>
-      <c r="Q31" s="242"/>
+      <c r="Q31" s="244"/>
       <c r="R31" s="6" t="s">
         <v>37</v>
       </c>
@@ -8782,7 +8857,7 @@
         <v>105</v>
       </c>
       <c r="O32" s="178"/>
-      <c r="Q32" s="242"/>
+      <c r="Q32" s="244"/>
       <c r="R32" s="23" t="s">
         <v>38</v>
       </c>
@@ -8797,7 +8872,7 @@
       </c>
     </row>
     <row r="33" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q33" s="242"/>
+      <c r="Q33" s="244"/>
       <c r="R33" s="23" t="s">
         <v>40</v>
       </c>
@@ -8810,7 +8885,7 @@
       <c r="U33" s="25"/>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q34" s="242"/>
+      <c r="Q34" s="244"/>
       <c r="R34" s="23" t="s">
         <v>42</v>
       </c>
@@ -8826,7 +8901,7 @@
       </c>
     </row>
     <row r="35" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q35" s="242"/>
+      <c r="Q35" s="244"/>
       <c r="R35" s="23" t="s">
         <v>34</v>
       </c>
@@ -8839,7 +8914,7 @@
       <c r="U35" s="25"/>
     </row>
     <row r="36" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q36" s="242"/>
+      <c r="Q36" s="244"/>
       <c r="R36" s="23" t="s">
         <v>36</v>
       </c>
@@ -8853,7 +8928,7 @@
       <c r="U36" s="190"/>
     </row>
     <row r="37" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q37" s="242"/>
+      <c r="Q37" s="244"/>
       <c r="R37" s="6" t="s">
         <v>44</v>
       </c>
@@ -8862,7 +8937,7 @@
       <c r="U37" s="30"/>
     </row>
     <row r="38" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q38" s="242"/>
+      <c r="Q38" s="244"/>
       <c r="R38" s="23" t="s">
         <v>45</v>
       </c>
@@ -8878,7 +8953,7 @@
       </c>
     </row>
     <row r="39" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q39" s="242"/>
+      <c r="Q39" s="244"/>
       <c r="R39" s="23" t="s">
         <v>46</v>
       </c>
@@ -8891,7 +8966,7 @@
       <c r="U39" s="25"/>
     </row>
     <row r="40" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="242"/>
+      <c r="Q40" s="244"/>
       <c r="R40" s="23" t="s">
         <v>34</v>
       </c>
@@ -8906,7 +8981,7 @@
       </c>
     </row>
     <row r="41" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="243"/>
+      <c r="Q41" s="245"/>
       <c r="R41" s="23" t="s">
         <v>36</v>
       </c>
@@ -8919,7 +8994,7 @@
       <c r="U41" s="22"/>
     </row>
     <row r="42" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q42" s="245" t="s">
+      <c r="Q42" s="247" t="s">
         <v>50</v>
       </c>
       <c r="R42" s="6" t="s">
@@ -8932,7 +9007,7 @@
       <c r="U42" s="30"/>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q43" s="233"/>
+      <c r="Q43" s="235"/>
       <c r="R43" s="6" t="s">
         <v>52</v>
       </c>
@@ -8941,7 +9016,7 @@
       <c r="U43" s="30"/>
     </row>
     <row r="44" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q44" s="233"/>
+      <c r="Q44" s="235"/>
       <c r="R44" s="23" t="s">
         <v>53</v>
       </c>
@@ -8952,7 +9027,7 @@
       <c r="U44" s="25"/>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q45" s="233"/>
+      <c r="Q45" s="235"/>
       <c r="R45" s="23" t="s">
         <v>54</v>
       </c>
@@ -8967,7 +9042,7 @@
       </c>
     </row>
     <row r="46" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q46" s="233"/>
+      <c r="Q46" s="235"/>
       <c r="R46" s="23" t="s">
         <v>57</v>
       </c>
@@ -8982,7 +9057,7 @@
       </c>
     </row>
     <row r="47" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q47" s="233"/>
+      <c r="Q47" s="235"/>
       <c r="R47" s="23" t="s">
         <v>59</v>
       </c>
@@ -8998,7 +9073,7 @@
       </c>
     </row>
     <row r="48" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q48" s="233"/>
+      <c r="Q48" s="235"/>
       <c r="R48" s="23"/>
       <c r="S48" s="26" t="s">
         <v>306</v>
@@ -9010,7 +9085,7 @@
       <c r="U48" s="25"/>
     </row>
     <row r="49" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q49" s="233"/>
+      <c r="Q49" s="235"/>
       <c r="R49" s="23" t="s">
         <v>61</v>
       </c>
@@ -9024,7 +9099,7 @@
       <c r="U49" s="25"/>
     </row>
     <row r="50" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q50" s="233"/>
+      <c r="Q50" s="235"/>
       <c r="R50" s="6" t="s">
         <v>62</v>
       </c>
@@ -9036,7 +9111,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="Q51" s="233"/>
+      <c r="Q51" s="235"/>
       <c r="R51" s="23" t="s">
         <v>63</v>
       </c>
@@ -9051,7 +9126,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="N52" s="144"/>
-      <c r="Q52" s="233"/>
+      <c r="Q52" s="235"/>
       <c r="R52" s="23" t="s">
         <v>54</v>
       </c>
@@ -9069,7 +9144,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
-      <c r="Q53" s="233"/>
+      <c r="Q53" s="235"/>
       <c r="R53" s="23" t="s">
         <v>64</v>
       </c>
@@ -9085,7 +9160,7 @@
       </c>
     </row>
     <row r="54" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q54" s="233"/>
+      <c r="Q54" s="235"/>
       <c r="R54" s="23" t="s">
         <v>66</v>
       </c>
@@ -9101,7 +9176,7 @@
       </c>
     </row>
     <row r="55" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q55" s="233"/>
+      <c r="Q55" s="235"/>
       <c r="R55" s="23" t="s">
         <v>61</v>
       </c>
@@ -9115,7 +9190,7 @@
       <c r="U55" s="25"/>
     </row>
     <row r="56" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q56" s="233"/>
+      <c r="Q56" s="235"/>
       <c r="R56" s="6" t="s">
         <v>69</v>
       </c>
@@ -9124,7 +9199,7 @@
       <c r="U56" s="30"/>
     </row>
     <row r="57" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q57" s="233"/>
+      <c r="Q57" s="235"/>
       <c r="R57" s="23" t="s">
         <v>70</v>
       </c>
@@ -9135,7 +9210,7 @@
       <c r="U57" s="25"/>
     </row>
     <row r="58" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q58" s="233"/>
+      <c r="Q58" s="235"/>
       <c r="R58" s="23" t="s">
         <v>54</v>
       </c>
@@ -9151,7 +9226,7 @@
       <c r="V58" s="27"/>
     </row>
     <row r="59" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q59" s="233"/>
+      <c r="Q59" s="235"/>
       <c r="R59" s="23" t="s">
         <v>57</v>
       </c>
@@ -9166,7 +9241,7 @@
       </c>
     </row>
     <row r="60" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q60" s="233"/>
+      <c r="Q60" s="235"/>
       <c r="R60" s="23" t="s">
         <v>71</v>
       </c>
@@ -9179,7 +9254,7 @@
       <c r="U60" s="25"/>
     </row>
     <row r="61" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q61" s="233"/>
+      <c r="Q61" s="235"/>
       <c r="R61" s="23" t="s">
         <v>59</v>
       </c>
@@ -9196,7 +9271,7 @@
       <c r="V61" s="37"/>
     </row>
     <row r="62" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q62" s="233"/>
+      <c r="Q62" s="235"/>
       <c r="R62" s="23" t="s">
         <v>61</v>
       </c>
@@ -9211,7 +9286,7 @@
       <c r="V62" s="194"/>
     </row>
     <row r="63" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q63" s="233"/>
+      <c r="Q63" s="235"/>
       <c r="R63" s="6" t="s">
         <v>73</v>
       </c>
@@ -9220,7 +9295,7 @@
       <c r="U63" s="30"/>
     </row>
     <row r="64" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q64" s="233"/>
+      <c r="Q64" s="235"/>
       <c r="R64" s="23" t="s">
         <v>74</v>
       </c>
@@ -9235,7 +9310,7 @@
       </c>
     </row>
     <row r="65" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q65" s="234"/>
+      <c r="Q65" s="236"/>
       <c r="R65" s="40" t="s">
         <v>77</v>
       </c>
@@ -9250,7 +9325,7 @@
       </c>
     </row>
     <row r="66" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q66" s="232" t="s">
+      <c r="Q66" s="234" t="s">
         <v>346</v>
       </c>
       <c r="R66" s="18" t="s">
@@ -9263,7 +9338,7 @@
       <c r="U66" s="21"/>
     </row>
     <row r="67" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q67" s="233"/>
+      <c r="Q67" s="235"/>
       <c r="R67" s="6" t="s">
         <v>83</v>
       </c>
@@ -9272,7 +9347,7 @@
       <c r="U67" s="30"/>
     </row>
     <row r="68" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q68" s="233"/>
+      <c r="Q68" s="235"/>
       <c r="R68" s="23" t="s">
         <v>81</v>
       </c>
@@ -9285,7 +9360,7 @@
       <c r="U68" s="45"/>
     </row>
     <row r="69" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q69" s="233"/>
+      <c r="Q69" s="235"/>
       <c r="R69" s="2" t="s">
         <v>86</v>
       </c>
@@ -9298,7 +9373,7 @@
       </c>
     </row>
     <row r="70" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q70" s="233"/>
+      <c r="Q70" s="235"/>
       <c r="R70" s="6" t="s">
         <v>84</v>
       </c>
@@ -9307,7 +9382,7 @@
       <c r="U70" s="49"/>
     </row>
     <row r="71" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q71" s="233"/>
+      <c r="Q71" s="235"/>
       <c r="R71" s="23" t="s">
         <v>85</v>
       </c>
@@ -9320,7 +9395,7 @@
       <c r="U71" s="45"/>
     </row>
     <row r="72" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q72" s="233"/>
+      <c r="Q72" s="235"/>
       <c r="R72" s="23" t="s">
         <v>89</v>
       </c>
@@ -9335,7 +9410,7 @@
       </c>
     </row>
     <row r="73" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q73" s="234"/>
+      <c r="Q73" s="236"/>
       <c r="R73" s="40"/>
       <c r="S73" s="41" t="s">
         <v>88</v>
@@ -9393,20 +9468,20 @@
   <sheetData>
     <row r="1" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="235" t="s">
+      <c r="J2" s="237" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="236"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="236"/>
-      <c r="N2" s="237"/>
-      <c r="Q2" s="235" t="s">
+      <c r="K2" s="238"/>
+      <c r="L2" s="238"/>
+      <c r="M2" s="238"/>
+      <c r="N2" s="239"/>
+      <c r="Q2" s="237" t="s">
         <v>336</v>
       </c>
-      <c r="R2" s="236"/>
-      <c r="S2" s="236"/>
-      <c r="T2" s="236"/>
-      <c r="U2" s="237"/>
+      <c r="R2" s="238"/>
+      <c r="S2" s="238"/>
+      <c r="T2" s="238"/>
+      <c r="U2" s="239"/>
     </row>
     <row r="3" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J3" s="11"/>
@@ -9418,7 +9493,7 @@
       <c r="N3" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="Q3" s="241" t="s">
+      <c r="Q3" s="243" t="s">
         <v>3</v>
       </c>
       <c r="R3" s="18" t="s">
@@ -9445,7 +9520,7 @@
         <f>M4/25.4</f>
         <v>52.5</v>
       </c>
-      <c r="Q4" s="242"/>
+      <c r="Q4" s="244"/>
       <c r="R4" s="1"/>
       <c r="S4" s="166"/>
       <c r="T4" s="2"/>
@@ -9465,7 +9540,7 @@
         <f>M5/25.4</f>
         <v>48.031496062992126</v>
       </c>
-      <c r="Q5" s="242"/>
+      <c r="Q5" s="244"/>
       <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
@@ -9487,7 +9562,7 @@
         <f t="shared" ref="N6:N7" si="0">M6/25.4</f>
         <v>6.0000000000000009</v>
       </c>
-      <c r="Q6" s="242"/>
+      <c r="Q6" s="244"/>
       <c r="R6" s="23" t="s">
         <v>6</v>
       </c>
@@ -9509,7 +9584,7 @@
         <f t="shared" si="0"/>
         <v>12.000000000000002</v>
       </c>
-      <c r="Q7" s="242"/>
+      <c r="Q7" s="244"/>
       <c r="R7" s="23" t="s">
         <v>7</v>
       </c>
@@ -9537,7 +9612,7 @@
         <f>M8/25.4</f>
         <v>9</v>
       </c>
-      <c r="Q8" s="242"/>
+      <c r="Q8" s="244"/>
       <c r="R8" s="23" t="s">
         <v>10</v>
       </c>
@@ -9562,7 +9637,7 @@
       <c r="N9" s="200" t="s">
         <v>352</v>
       </c>
-      <c r="Q9" s="242"/>
+      <c r="Q9" s="244"/>
       <c r="R9" s="3" t="s">
         <v>11</v>
       </c>
@@ -9575,7 +9650,7 @@
       <c r="U9" s="29"/>
     </row>
     <row r="10" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q10" s="242"/>
+      <c r="Q10" s="244"/>
       <c r="R10" s="6" t="s">
         <v>13</v>
       </c>
@@ -9584,14 +9659,14 @@
       <c r="U10" s="30"/>
     </row>
     <row r="11" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="238" t="s">
+      <c r="J11" s="240" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="239"/>
-      <c r="L11" s="239"/>
-      <c r="M11" s="239"/>
-      <c r="N11" s="240"/>
-      <c r="Q11" s="242"/>
+      <c r="K11" s="241"/>
+      <c r="L11" s="241"/>
+      <c r="M11" s="241"/>
+      <c r="N11" s="242"/>
+      <c r="Q11" s="244"/>
       <c r="R11" s="23" t="s">
         <v>6</v>
       </c>
@@ -9615,7 +9690,7 @@
       <c r="N12" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="Q12" s="242"/>
+      <c r="Q12" s="244"/>
       <c r="R12" s="23" t="s">
         <v>7</v>
       </c>
@@ -9648,7 +9723,7 @@
         <f>M13/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="242"/>
+      <c r="Q13" s="244"/>
       <c r="R13" s="23" t="s">
         <v>10</v>
       </c>
@@ -9677,7 +9752,7 @@
         <f t="shared" ref="N14:N32" si="2">M14/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="242"/>
+      <c r="Q14" s="244"/>
       <c r="R14" s="3" t="s">
         <v>11</v>
       </c>
@@ -9709,7 +9784,7 @@
         <v>6.2143700787401581</v>
       </c>
       <c r="O15" s="178"/>
-      <c r="Q15" s="242"/>
+      <c r="Q15" s="244"/>
       <c r="R15" s="6" t="s">
         <v>16</v>
       </c>
@@ -9736,7 +9811,7 @@
         <f t="shared" si="2"/>
         <v>6.2143700787401581</v>
       </c>
-      <c r="Q16" s="242"/>
+      <c r="Q16" s="244"/>
       <c r="R16" s="23" t="s">
         <v>6</v>
       </c>
@@ -9764,7 +9839,7 @@
         <v>12.428543307086615</v>
       </c>
       <c r="O17" s="178"/>
-      <c r="Q17" s="242"/>
+      <c r="Q17" s="244"/>
       <c r="R17" s="23" t="s">
         <v>7</v>
       </c>
@@ -9797,7 +9872,7 @@
         <f t="shared" si="2"/>
         <v>12.428543307086615</v>
       </c>
-      <c r="Q18" s="242"/>
+      <c r="Q18" s="244"/>
       <c r="R18" s="23" t="s">
         <v>10</v>
       </c>
@@ -9827,7 +9902,7 @@
         <v>18.642913385826773</v>
       </c>
       <c r="O19" s="178"/>
-      <c r="Q19" s="242"/>
+      <c r="Q19" s="244"/>
       <c r="R19" s="3" t="s">
         <v>11</v>
       </c>
@@ -9859,7 +9934,7 @@
         <f t="shared" si="2"/>
         <v>18.642913385826773</v>
       </c>
-      <c r="Q20" s="242"/>
+      <c r="Q20" s="244"/>
       <c r="R20" s="32" t="s">
         <v>19</v>
       </c>
@@ -9893,7 +9968,7 @@
         <v>24.85708661417323</v>
       </c>
       <c r="O21" s="178"/>
-      <c r="Q21" s="242"/>
+      <c r="Q21" s="244"/>
       <c r="R21" s="32" t="s">
         <v>21</v>
       </c>
@@ -9924,7 +9999,7 @@
         <f t="shared" si="2"/>
         <v>24.85708661417323</v>
       </c>
-      <c r="Q22" s="242"/>
+      <c r="Q22" s="244"/>
       <c r="R22" s="32" t="s">
         <v>24</v>
       </c>
@@ -9956,7 +10031,7 @@
         <v>31.07145669291339</v>
       </c>
       <c r="O23" s="178"/>
-      <c r="Q23" s="243"/>
+      <c r="Q23" s="245"/>
       <c r="R23" s="2"/>
       <c r="S23" s="8" t="s">
         <v>26</v>
@@ -9985,7 +10060,7 @@
         <f t="shared" si="2"/>
         <v>31.07145669291339</v>
       </c>
-      <c r="Q24" s="244" t="s">
+      <c r="Q24" s="246" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -10017,7 +10092,7 @@
         <v>37.28562992125984</v>
       </c>
       <c r="O25" s="178"/>
-      <c r="Q25" s="242"/>
+      <c r="Q25" s="244"/>
       <c r="R25" s="6" t="s">
         <v>29</v>
       </c>
@@ -10044,7 +10119,7 @@
         <f t="shared" si="2"/>
         <v>37.28562992125984</v>
       </c>
-      <c r="Q26" s="242"/>
+      <c r="Q26" s="244"/>
       <c r="R26" s="23" t="s">
         <v>30</v>
       </c>
@@ -10078,7 +10153,7 @@
         <v>43.500000000000007</v>
       </c>
       <c r="O27" s="178"/>
-      <c r="Q27" s="242"/>
+      <c r="Q27" s="244"/>
       <c r="R27" s="23" t="s">
         <v>32</v>
       </c>
@@ -10109,7 +10184,7 @@
         <f t="shared" si="2"/>
         <v>43.500000000000007</v>
       </c>
-      <c r="Q28" s="242"/>
+      <c r="Q28" s="244"/>
       <c r="R28" s="23" t="s">
         <v>19</v>
       </c>
@@ -10144,7 +10219,7 @@
         <v>48.000000000000007</v>
       </c>
       <c r="O29" s="178"/>
-      <c r="Q29" s="242"/>
+      <c r="Q29" s="244"/>
       <c r="R29" s="23" t="s">
         <v>34</v>
       </c>
@@ -10176,7 +10251,7 @@
         <f t="shared" si="2"/>
         <v>48.000000000000007</v>
       </c>
-      <c r="Q30" s="242"/>
+      <c r="Q30" s="244"/>
       <c r="R30" s="23" t="s">
         <v>36</v>
       </c>
@@ -10209,7 +10284,7 @@
         <v>52.5</v>
       </c>
       <c r="O31" s="178"/>
-      <c r="Q31" s="242"/>
+      <c r="Q31" s="244"/>
       <c r="R31" s="6" t="s">
         <v>37</v>
       </c>
@@ -10236,7 +10311,7 @@
         <f t="shared" si="2"/>
         <v>52.5</v>
       </c>
-      <c r="Q32" s="242"/>
+      <c r="Q32" s="244"/>
       <c r="R32" s="23" t="s">
         <v>38</v>
       </c>
@@ -10251,7 +10326,7 @@
       </c>
     </row>
     <row r="33" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q33" s="242"/>
+      <c r="Q33" s="244"/>
       <c r="R33" s="23" t="s">
         <v>40</v>
       </c>
@@ -10264,7 +10339,7 @@
       <c r="U33" s="25"/>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q34" s="242"/>
+      <c r="Q34" s="244"/>
       <c r="R34" s="23" t="s">
         <v>42</v>
       </c>
@@ -10280,7 +10355,7 @@
       </c>
     </row>
     <row r="35" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q35" s="242"/>
+      <c r="Q35" s="244"/>
       <c r="R35" s="23" t="s">
         <v>34</v>
       </c>
@@ -10293,7 +10368,7 @@
       <c r="U35" s="25"/>
     </row>
     <row r="36" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q36" s="242"/>
+      <c r="Q36" s="244"/>
       <c r="R36" s="23" t="s">
         <v>36</v>
       </c>
@@ -10307,7 +10382,7 @@
       <c r="U36" s="190"/>
     </row>
     <row r="37" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q37" s="242"/>
+      <c r="Q37" s="244"/>
       <c r="R37" s="6" t="s">
         <v>44</v>
       </c>
@@ -10316,7 +10391,7 @@
       <c r="U37" s="30"/>
     </row>
     <row r="38" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q38" s="242"/>
+      <c r="Q38" s="244"/>
       <c r="R38" s="23" t="s">
         <v>45</v>
       </c>
@@ -10332,7 +10407,7 @@
       </c>
     </row>
     <row r="39" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q39" s="242"/>
+      <c r="Q39" s="244"/>
       <c r="R39" s="23" t="s">
         <v>46</v>
       </c>
@@ -10345,7 +10420,7 @@
       <c r="U39" s="25"/>
     </row>
     <row r="40" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="242"/>
+      <c r="Q40" s="244"/>
       <c r="R40" s="23" t="s">
         <v>34</v>
       </c>
@@ -10360,7 +10435,7 @@
       </c>
     </row>
     <row r="41" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="243"/>
+      <c r="Q41" s="245"/>
       <c r="R41" s="23" t="s">
         <v>36</v>
       </c>
@@ -10373,7 +10448,7 @@
       <c r="U41" s="22"/>
     </row>
     <row r="42" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q42" s="245" t="s">
+      <c r="Q42" s="247" t="s">
         <v>50</v>
       </c>
       <c r="R42" s="6" t="s">
@@ -10386,7 +10461,7 @@
       <c r="U42" s="30"/>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q43" s="233"/>
+      <c r="Q43" s="235"/>
       <c r="R43" s="6" t="s">
         <v>52</v>
       </c>
@@ -10395,7 +10470,7 @@
       <c r="U43" s="30"/>
     </row>
     <row r="44" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q44" s="233"/>
+      <c r="Q44" s="235"/>
       <c r="R44" s="23" t="s">
         <v>53</v>
       </c>
@@ -10406,7 +10481,7 @@
       <c r="U44" s="25"/>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q45" s="233"/>
+      <c r="Q45" s="235"/>
       <c r="R45" s="23" t="s">
         <v>54</v>
       </c>
@@ -10421,7 +10496,7 @@
       </c>
     </row>
     <row r="46" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q46" s="233"/>
+      <c r="Q46" s="235"/>
       <c r="R46" s="23" t="s">
         <v>57</v>
       </c>
@@ -10436,7 +10511,7 @@
       </c>
     </row>
     <row r="47" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q47" s="233"/>
+      <c r="Q47" s="235"/>
       <c r="R47" s="23" t="s">
         <v>59</v>
       </c>
@@ -10452,7 +10527,7 @@
       </c>
     </row>
     <row r="48" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q48" s="233"/>
+      <c r="Q48" s="235"/>
       <c r="R48" s="23"/>
       <c r="S48" s="26" t="s">
         <v>306</v>
@@ -10464,7 +10539,7 @@
       <c r="U48" s="25"/>
     </row>
     <row r="49" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q49" s="233"/>
+      <c r="Q49" s="235"/>
       <c r="R49" s="23" t="s">
         <v>61</v>
       </c>
@@ -10478,7 +10553,7 @@
       <c r="U49" s="25"/>
     </row>
     <row r="50" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q50" s="233"/>
+      <c r="Q50" s="235"/>
       <c r="R50" s="6" t="s">
         <v>62</v>
       </c>
@@ -10490,7 +10565,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="Q51" s="233"/>
+      <c r="Q51" s="235"/>
       <c r="R51" s="23" t="s">
         <v>63</v>
       </c>
@@ -10505,7 +10580,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="N52" s="144"/>
-      <c r="Q52" s="233"/>
+      <c r="Q52" s="235"/>
       <c r="R52" s="23" t="s">
         <v>54</v>
       </c>
@@ -10523,7 +10598,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
-      <c r="Q53" s="233"/>
+      <c r="Q53" s="235"/>
       <c r="R53" s="23" t="s">
         <v>64</v>
       </c>
@@ -10539,7 +10614,7 @@
       </c>
     </row>
     <row r="54" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q54" s="233"/>
+      <c r="Q54" s="235"/>
       <c r="R54" s="23" t="s">
         <v>66</v>
       </c>
@@ -10555,7 +10630,7 @@
       </c>
     </row>
     <row r="55" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q55" s="233"/>
+      <c r="Q55" s="235"/>
       <c r="R55" s="23" t="s">
         <v>61</v>
       </c>
@@ -10569,7 +10644,7 @@
       <c r="U55" s="25"/>
     </row>
     <row r="56" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q56" s="233"/>
+      <c r="Q56" s="235"/>
       <c r="R56" s="6" t="s">
         <v>69</v>
       </c>
@@ -10578,7 +10653,7 @@
       <c r="U56" s="30"/>
     </row>
     <row r="57" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q57" s="233"/>
+      <c r="Q57" s="235"/>
       <c r="R57" s="23" t="s">
         <v>70</v>
       </c>
@@ -10589,7 +10664,7 @@
       <c r="U57" s="25"/>
     </row>
     <row r="58" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q58" s="233"/>
+      <c r="Q58" s="235"/>
       <c r="R58" s="23" t="s">
         <v>54</v>
       </c>
@@ -10605,7 +10680,7 @@
       <c r="V58" s="27"/>
     </row>
     <row r="59" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q59" s="233"/>
+      <c r="Q59" s="235"/>
       <c r="R59" s="23" t="s">
         <v>57</v>
       </c>
@@ -10620,7 +10695,7 @@
       </c>
     </row>
     <row r="60" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q60" s="233"/>
+      <c r="Q60" s="235"/>
       <c r="R60" s="23" t="s">
         <v>71</v>
       </c>
@@ -10633,7 +10708,7 @@
       <c r="U60" s="25"/>
     </row>
     <row r="61" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q61" s="233"/>
+      <c r="Q61" s="235"/>
       <c r="R61" s="23" t="s">
         <v>59</v>
       </c>
@@ -10650,7 +10725,7 @@
       <c r="V61" s="37"/>
     </row>
     <row r="62" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q62" s="233"/>
+      <c r="Q62" s="235"/>
       <c r="R62" s="23" t="s">
         <v>61</v>
       </c>
@@ -10665,7 +10740,7 @@
       <c r="V62" s="194"/>
     </row>
     <row r="63" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q63" s="233"/>
+      <c r="Q63" s="235"/>
       <c r="R63" s="6" t="s">
         <v>73</v>
       </c>
@@ -10674,7 +10749,7 @@
       <c r="U63" s="30"/>
     </row>
     <row r="64" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q64" s="233"/>
+      <c r="Q64" s="235"/>
       <c r="R64" s="23" t="s">
         <v>74</v>
       </c>
@@ -10689,7 +10764,7 @@
       </c>
     </row>
     <row r="65" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q65" s="234"/>
+      <c r="Q65" s="236"/>
       <c r="R65" s="40" t="s">
         <v>77</v>
       </c>
@@ -10704,7 +10779,7 @@
       </c>
     </row>
     <row r="66" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q66" s="232" t="s">
+      <c r="Q66" s="234" t="s">
         <v>346</v>
       </c>
       <c r="R66" s="18" t="s">
@@ -10717,7 +10792,7 @@
       <c r="U66" s="21"/>
     </row>
     <row r="67" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q67" s="233"/>
+      <c r="Q67" s="235"/>
       <c r="R67" s="6" t="s">
         <v>83</v>
       </c>
@@ -10726,7 +10801,7 @@
       <c r="U67" s="30"/>
     </row>
     <row r="68" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q68" s="233"/>
+      <c r="Q68" s="235"/>
       <c r="R68" s="23" t="s">
         <v>81</v>
       </c>
@@ -10739,7 +10814,7 @@
       <c r="U68" s="45"/>
     </row>
     <row r="69" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q69" s="233"/>
+      <c r="Q69" s="235"/>
       <c r="R69" s="2" t="s">
         <v>86</v>
       </c>
@@ -10752,7 +10827,7 @@
       </c>
     </row>
     <row r="70" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q70" s="233"/>
+      <c r="Q70" s="235"/>
       <c r="R70" s="6" t="s">
         <v>84</v>
       </c>
@@ -10761,7 +10836,7 @@
       <c r="U70" s="49"/>
     </row>
     <row r="71" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q71" s="233"/>
+      <c r="Q71" s="235"/>
       <c r="R71" s="23" t="s">
         <v>85</v>
       </c>
@@ -10774,7 +10849,7 @@
       <c r="U71" s="45"/>
     </row>
     <row r="72" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q72" s="233"/>
+      <c r="Q72" s="235"/>
       <c r="R72" s="23" t="s">
         <v>89</v>
       </c>
@@ -10789,7 +10864,7 @@
       </c>
     </row>
     <row r="73" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q73" s="234"/>
+      <c r="Q73" s="236"/>
       <c r="R73" s="40"/>
       <c r="S73" s="41" t="s">
         <v>88</v>
@@ -10821,10 +10896,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE64495-0A64-4917-8E7B-BBB41A05E68F}">
-  <dimension ref="I3:Z33"/>
+  <dimension ref="H3:Z66"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" topLeftCell="E42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10847,13 +10922,13 @@
   <sheetData>
     <row r="3" spans="9:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="9:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I4" s="238" t="s">
+      <c r="I4" s="240" t="s">
         <v>80</v>
       </c>
-      <c r="J4" s="239"/>
-      <c r="K4" s="239"/>
-      <c r="L4" s="239"/>
-      <c r="M4" s="240"/>
+      <c r="J4" s="241"/>
+      <c r="K4" s="241"/>
+      <c r="L4" s="241"/>
+      <c r="M4" s="242"/>
     </row>
     <row r="5" spans="9:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I5" s="11" t="s">
@@ -10871,13 +10946,13 @@
       <c r="M5" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="P5" s="238" t="s">
+      <c r="P5" s="240" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="239"/>
-      <c r="R5" s="239"/>
-      <c r="S5" s="239"/>
-      <c r="T5" s="240"/>
+      <c r="Q5" s="241"/>
+      <c r="R5" s="241"/>
+      <c r="S5" s="241"/>
+      <c r="T5" s="242"/>
     </row>
     <row r="6" spans="9:26" x14ac:dyDescent="0.3">
       <c r="I6" s="14">
@@ -11423,7 +11498,7 @@
       </c>
     </row>
     <row r="18" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I18" s="281">
+      <c r="I18" s="232">
         <v>13</v>
       </c>
       <c r="J18" s="198">
@@ -11437,7 +11512,7 @@
         <f t="shared" si="1"/>
         <v>2438.3999999999996</v>
       </c>
-      <c r="M18" s="282">
+      <c r="M18" s="233">
         <f>M17+N18</f>
         <v>96</v>
       </c>
@@ -11470,7 +11545,7 @@
       </c>
     </row>
     <row r="19" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I19" s="281">
+      <c r="I19" s="232">
         <v>14</v>
       </c>
       <c r="J19" s="198">
@@ -11484,7 +11559,7 @@
         <f>M19*25.4</f>
         <v>2438.3999999999996</v>
       </c>
-      <c r="M19" s="282">
+      <c r="M19" s="233">
         <f>M18</f>
         <v>96</v>
       </c>
@@ -11587,10 +11662,12 @@
         <f t="shared" si="3"/>
         <v>87.000000000000014</v>
       </c>
-      <c r="V21">
+      <c r="V21" s="283">
         <v>15</v>
       </c>
-      <c r="Y21">
+      <c r="W21" s="283"/>
+      <c r="X21" s="283"/>
+      <c r="Y21" s="283">
         <f>Y19+S33</f>
         <v>2438.4</v>
       </c>
@@ -11628,10 +11705,12 @@
         <f t="shared" si="3"/>
         <v>87.000000000000014</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="283">
         <v>16</v>
       </c>
-      <c r="Y22">
+      <c r="W22" s="283"/>
+      <c r="X22" s="283"/>
+      <c r="Y22" s="283">
         <f>Y21</f>
         <v>2438.4</v>
       </c>
@@ -11652,7 +11731,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="179"/>
-      <c r="P23" s="281">
+      <c r="P23" s="232">
         <v>17</v>
       </c>
       <c r="Q23" s="198">
@@ -11665,7 +11744,7 @@
       <c r="S23" s="198">
         <v>2438.4</v>
       </c>
-      <c r="T23" s="282">
+      <c r="T23" s="233">
         <f t="shared" si="3"/>
         <v>96.000000000000014</v>
       </c>
@@ -11693,7 +11772,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="179"/>
-      <c r="P24" s="281">
+      <c r="P24" s="232">
         <v>18</v>
       </c>
       <c r="Q24" s="198">
@@ -11706,7 +11785,7 @@
       <c r="S24" s="198">
         <v>2438.4</v>
       </c>
-      <c r="T24" s="282">
+      <c r="T24" s="233">
         <f t="shared" si="3"/>
         <v>96.000000000000014</v>
       </c>
@@ -11780,6 +11859,106 @@
     <row r="33" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S33">
         <v>228.6</v>
+      </c>
+    </row>
+    <row r="58" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H58" t="s">
+        <v>376</v>
+      </c>
+      <c r="J58" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="59" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I59">
+        <v>47.09</v>
+      </c>
+      <c r="J59">
+        <v>53.78</v>
+      </c>
+    </row>
+    <row r="60" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H60" t="s">
+        <v>372</v>
+      </c>
+      <c r="I60">
+        <v>2.32E-3</v>
+      </c>
+      <c r="J60">
+        <v>3.9699999999999996E-3</v>
+      </c>
+      <c r="N60" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="61" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H61" t="s">
+        <v>375</v>
+      </c>
+      <c r="I61">
+        <f>4700*I59^0.5</f>
+        <v>32252.412312879791</v>
+      </c>
+      <c r="J61">
+        <f>4700*J59^0.5</f>
+        <v>34467.378780522318</v>
+      </c>
+      <c r="N61" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H62" t="s">
+        <v>373</v>
+      </c>
+      <c r="I62">
+        <v>610</v>
+      </c>
+      <c r="J62">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="63" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H63" t="s">
+        <v>378</v>
+      </c>
+      <c r="I63" t="s">
+        <v>379</v>
+      </c>
+      <c r="J63">
+        <f>5*(J59/I59-0.85)</f>
+        <v>1.4603418984922483</v>
+      </c>
+    </row>
+    <row r="64" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H64" t="s">
+        <v>370</v>
+      </c>
+      <c r="I64">
+        <v>87.563000000000002</v>
+      </c>
+      <c r="J64">
+        <f>J63*I64</f>
+        <v>127.87191765767673</v>
+      </c>
+      <c r="N64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H66" t="s">
+        <v>374</v>
+      </c>
+      <c r="I66">
+        <f>I60-I59/I61+2*(I64/I62)/I59</f>
+        <v>6.9566159544933127E-3</v>
+      </c>
+      <c r="J66">
+        <f>J60-0.8*J59/J61+((5/3)*J64/J62)/I59</f>
+        <v>1.0141089460168916E-2</v>
       </c>
     </row>
   </sheetData>
@@ -11812,10 +11991,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="249" t="s">
+      <c r="C3" s="251" t="s">
         <v>215</v>
       </c>
-      <c r="D3" s="249" t="s">
+      <c r="D3" s="251" t="s">
         <v>91</v>
       </c>
       <c r="E3" s="82">
@@ -11827,8 +12006,8 @@
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="249"/>
-      <c r="D4" s="249"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
       <c r="E4" s="84">
         <f>E3*9.807</f>
         <v>-2145185.2167177605</v>
@@ -11842,7 +12021,7 @@
       </c>
     </row>
     <row r="8" spans="3:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="250">
+      <c r="C8" s="252">
         <v>1</v>
       </c>
       <c r="D8" s="147" t="s">
@@ -11855,7 +12034,7 @@
       <c r="G8" s="150"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="251"/>
+      <c r="C9" s="253"/>
       <c r="D9" s="151" t="s">
         <v>111</v>
       </c>
@@ -11864,7 +12043,7 @@
       <c r="G9" s="153"/>
     </row>
     <row r="10" spans="3:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C10" s="251"/>
+      <c r="C10" s="253"/>
       <c r="D10" s="154" t="s">
         <v>34</v>
       </c>
@@ -11877,7 +12056,7 @@
       <c r="G10" s="157"/>
     </row>
     <row r="11" spans="3:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C11" s="251"/>
+      <c r="C11" s="253"/>
       <c r="D11" s="151" t="s">
         <v>113</v>
       </c>
@@ -11886,7 +12065,7 @@
       <c r="G11" s="157"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="251"/>
+      <c r="C12" s="253"/>
       <c r="D12" s="154" t="s">
         <v>114</v>
       </c>
@@ -11899,7 +12078,7 @@
       <c r="G12" s="153"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="251"/>
+      <c r="C13" s="253"/>
       <c r="D13" s="151" t="s">
         <v>112</v>
       </c>
@@ -11911,7 +12090,7 @@
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="251"/>
+      <c r="C14" s="253"/>
       <c r="D14" s="154" t="s">
         <v>98</v>
       </c>
@@ -11928,7 +12107,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="251"/>
+      <c r="C15" s="253"/>
       <c r="D15" s="154" t="s">
         <v>97</v>
       </c>
@@ -11948,7 +12127,7 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="251"/>
+      <c r="C16" s="253"/>
       <c r="D16" s="154" t="s">
         <v>102</v>
       </c>
@@ -11961,7 +12140,7 @@
       <c r="G16" s="153"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="251"/>
+      <c r="C17" s="253"/>
       <c r="D17" s="154" t="s">
         <v>103</v>
       </c>
@@ -11974,7 +12153,7 @@
       <c r="G17" s="153"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="251"/>
+      <c r="C18" s="253"/>
       <c r="D18" s="154" t="s">
         <v>94</v>
       </c>
@@ -11987,7 +12166,7 @@
       <c r="G18" s="153"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="251"/>
+      <c r="C19" s="253"/>
       <c r="D19" s="161" t="s">
         <v>95</v>
       </c>
@@ -12000,7 +12179,7 @@
       <c r="G19" s="164"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="251"/>
+      <c r="C20" s="253"/>
       <c r="D20" s="147" t="s">
         <v>116</v>
       </c>
@@ -12011,7 +12190,7 @@
       <c r="G20" s="150"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="251"/>
+      <c r="C21" s="253"/>
       <c r="D21" s="154" t="s">
         <v>119</v>
       </c>
@@ -12022,7 +12201,7 @@
       <c r="G21" s="153"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="251"/>
+      <c r="C22" s="253"/>
       <c r="D22" s="161" t="s">
         <v>121</v>
       </c>
@@ -12033,7 +12212,7 @@
       <c r="G22" s="164"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="251"/>
+      <c r="C23" s="253"/>
       <c r="D23" s="147" t="s">
         <v>116</v>
       </c>
@@ -12044,7 +12223,7 @@
       <c r="G23" s="150"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="251"/>
+      <c r="C24" s="253"/>
       <c r="D24" s="154" t="s">
         <v>126</v>
       </c>
@@ -12057,7 +12236,7 @@
       <c r="G24" s="153"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="251"/>
+      <c r="C25" s="253"/>
       <c r="D25" s="154" t="s">
         <v>119</v>
       </c>
@@ -12070,7 +12249,7 @@
       <c r="G25" s="153"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="252"/>
+      <c r="C26" s="254"/>
       <c r="D26" s="161" t="s">
         <v>110</v>
       </c>
@@ -12083,7 +12262,7 @@
       <c r="G26" s="164"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="246" t="s">
+      <c r="C27" s="248" t="s">
         <v>307</v>
       </c>
       <c r="D27" s="65" t="s">
@@ -12096,14 +12275,14 @@
       <c r="G27" s="68"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="247"/>
+      <c r="C28" s="249"/>
       <c r="D28" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C29" s="247"/>
+      <c r="C29" s="249"/>
       <c r="D29" s="56" t="s">
         <v>34</v>
       </c>
@@ -12116,7 +12295,7 @@
       <c r="G29" s="57"/>
     </row>
     <row r="30" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C30" s="247"/>
+      <c r="C30" s="249"/>
       <c r="D30" s="54" t="s">
         <v>113</v>
       </c>
@@ -12125,7 +12304,7 @@
       <c r="G30" s="57"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="247"/>
+      <c r="C31" s="249"/>
       <c r="D31" s="56" t="s">
         <v>114</v>
       </c>
@@ -12140,14 +12319,14 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="247"/>
+      <c r="C32" s="249"/>
       <c r="D32" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="247"/>
+      <c r="C33" s="249"/>
       <c r="D33" s="56" t="s">
         <v>98</v>
       </c>
@@ -12158,7 +12337,7 @@
       <c r="G33" s="55"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="247"/>
+      <c r="C34" s="249"/>
       <c r="D34" s="56" t="s">
         <v>97</v>
       </c>
@@ -12171,7 +12350,7 @@
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="247"/>
+      <c r="C35" s="249"/>
       <c r="D35" s="56" t="s">
         <v>102</v>
       </c>
@@ -12184,7 +12363,7 @@
       <c r="G35" s="55"/>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="247"/>
+      <c r="C36" s="249"/>
       <c r="D36" s="56" t="s">
         <v>103</v>
       </c>
@@ -12197,7 +12376,7 @@
       <c r="G36" s="55"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="247"/>
+      <c r="C37" s="249"/>
       <c r="D37" s="56" t="s">
         <v>94</v>
       </c>
@@ -12210,7 +12389,7 @@
       <c r="G37" s="55"/>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="247"/>
+      <c r="C38" s="249"/>
       <c r="D38" s="60" t="s">
         <v>95</v>
       </c>
@@ -12223,7 +12402,7 @@
       <c r="G38" s="63"/>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="247"/>
+      <c r="C39" s="249"/>
       <c r="D39" s="65" t="s">
         <v>116</v>
       </c>
@@ -12234,7 +12413,7 @@
       <c r="G39" s="68"/>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="247"/>
+      <c r="C40" s="249"/>
       <c r="D40" s="56" t="s">
         <v>119</v>
       </c>
@@ -12244,7 +12423,7 @@
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="247"/>
+      <c r="C41" s="249"/>
       <c r="D41" s="60" t="s">
         <v>121</v>
       </c>
@@ -12255,7 +12434,7 @@
       <c r="G41" s="63"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="247"/>
+      <c r="C42" s="249"/>
       <c r="D42" s="65" t="s">
         <v>116</v>
       </c>
@@ -12266,7 +12445,7 @@
       <c r="G42" s="68"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="247"/>
+      <c r="C43" s="249"/>
       <c r="D43" s="56" t="s">
         <v>126</v>
       </c>
@@ -12279,7 +12458,7 @@
       <c r="G43" s="55"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="247"/>
+      <c r="C44" s="249"/>
       <c r="D44" s="56" t="s">
         <v>119</v>
       </c>
@@ -12292,7 +12471,7 @@
       <c r="G44" s="55"/>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="248"/>
+      <c r="C45" s="250"/>
       <c r="D45" s="60" t="s">
         <v>110</v>
       </c>
@@ -12305,7 +12484,7 @@
       <c r="G45" s="63"/>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="246" t="s">
+      <c r="C46" s="248" t="s">
         <v>308</v>
       </c>
       <c r="D46" s="65" t="s">
@@ -12318,14 +12497,14 @@
       <c r="G46" s="68"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="247"/>
+      <c r="C47" s="249"/>
       <c r="D47" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G47" s="55"/>
     </row>
     <row r="48" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C48" s="247"/>
+      <c r="C48" s="249"/>
       <c r="D48" s="56" t="s">
         <v>34</v>
       </c>
@@ -12338,7 +12517,7 @@
       <c r="G48" s="57"/>
     </row>
     <row r="49" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C49" s="247"/>
+      <c r="C49" s="249"/>
       <c r="D49" s="54" t="s">
         <v>113</v>
       </c>
@@ -12347,7 +12526,7 @@
       <c r="G49" s="57"/>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="247"/>
+      <c r="C50" s="249"/>
       <c r="D50" s="56" t="s">
         <v>114</v>
       </c>
@@ -12362,14 +12541,14 @@
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="247"/>
+      <c r="C51" s="249"/>
       <c r="D51" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G51" s="55"/>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="247"/>
+      <c r="C52" s="249"/>
       <c r="D52" s="56" t="s">
         <v>98</v>
       </c>
@@ -12380,7 +12559,7 @@
       <c r="G52" s="55"/>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="247"/>
+      <c r="C53" s="249"/>
       <c r="D53" s="56" t="s">
         <v>97</v>
       </c>
@@ -12393,7 +12572,7 @@
       <c r="G53" s="55"/>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="247"/>
+      <c r="C54" s="249"/>
       <c r="D54" s="56" t="s">
         <v>102</v>
       </c>
@@ -12406,7 +12585,7 @@
       <c r="G54" s="55"/>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="247"/>
+      <c r="C55" s="249"/>
       <c r="D55" s="56" t="s">
         <v>103</v>
       </c>
@@ -12419,7 +12598,7 @@
       <c r="G55" s="55"/>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="247"/>
+      <c r="C56" s="249"/>
       <c r="D56" s="56" t="s">
         <v>94</v>
       </c>
@@ -12432,7 +12611,7 @@
       <c r="G56" s="55"/>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="247"/>
+      <c r="C57" s="249"/>
       <c r="D57" s="60" t="s">
         <v>95</v>
       </c>
@@ -12445,7 +12624,7 @@
       <c r="G57" s="63"/>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="247"/>
+      <c r="C58" s="249"/>
       <c r="D58" s="65" t="s">
         <v>116</v>
       </c>
@@ -12456,7 +12635,7 @@
       <c r="G58" s="68"/>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="247"/>
+      <c r="C59" s="249"/>
       <c r="D59" s="56" t="s">
         <v>119</v>
       </c>
@@ -12466,7 +12645,7 @@
       <c r="G59" s="55"/>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="247"/>
+      <c r="C60" s="249"/>
       <c r="D60" s="60" t="s">
         <v>121</v>
       </c>
@@ -12477,7 +12656,7 @@
       <c r="G60" s="63"/>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="247"/>
+      <c r="C61" s="249"/>
       <c r="D61" s="65" t="s">
         <v>116</v>
       </c>
@@ -12488,7 +12667,7 @@
       <c r="G61" s="68"/>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="247"/>
+      <c r="C62" s="249"/>
       <c r="D62" s="56" t="s">
         <v>126</v>
       </c>
@@ -12501,7 +12680,7 @@
       <c r="G62" s="55"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="247"/>
+      <c r="C63" s="249"/>
       <c r="D63" s="56" t="s">
         <v>119</v>
       </c>
@@ -12514,7 +12693,7 @@
       <c r="G63" s="55"/>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="248"/>
+      <c r="C64" s="250"/>
       <c r="D64" s="60" t="s">
         <v>110</v>
       </c>
@@ -12527,7 +12706,7 @@
       <c r="G64" s="63"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="246" t="s">
+      <c r="C65" s="248" t="s">
         <v>309</v>
       </c>
       <c r="D65" s="65" t="s">
@@ -12540,14 +12719,14 @@
       <c r="G65" s="68"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="247"/>
+      <c r="C66" s="249"/>
       <c r="D66" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G66" s="55"/>
     </row>
     <row r="67" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C67" s="247"/>
+      <c r="C67" s="249"/>
       <c r="D67" s="56" t="s">
         <v>34</v>
       </c>
@@ -12560,7 +12739,7 @@
       <c r="G67" s="57"/>
     </row>
     <row r="68" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C68" s="247"/>
+      <c r="C68" s="249"/>
       <c r="D68" s="54" t="s">
         <v>113</v>
       </c>
@@ -12569,7 +12748,7 @@
       <c r="G68" s="57"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="247"/>
+      <c r="C69" s="249"/>
       <c r="D69" s="56" t="s">
         <v>114</v>
       </c>
@@ -12585,14 +12764,14 @@
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="247"/>
+      <c r="C70" s="249"/>
       <c r="D70" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G70" s="55"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="247"/>
+      <c r="C71" s="249"/>
       <c r="D71" s="56" t="s">
         <v>98</v>
       </c>
@@ -12603,7 +12782,7 @@
       <c r="G71" s="55"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="247"/>
+      <c r="C72" s="249"/>
       <c r="D72" s="56" t="s">
         <v>97</v>
       </c>
@@ -12616,7 +12795,7 @@
       <c r="G72" s="55"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="247"/>
+      <c r="C73" s="249"/>
       <c r="D73" s="56" t="s">
         <v>102</v>
       </c>
@@ -12629,7 +12808,7 @@
       <c r="G73" s="55"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="247"/>
+      <c r="C74" s="249"/>
       <c r="D74" s="56" t="s">
         <v>103</v>
       </c>
@@ -12642,7 +12821,7 @@
       <c r="G74" s="55"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="247"/>
+      <c r="C75" s="249"/>
       <c r="D75" s="56" t="s">
         <v>94</v>
       </c>
@@ -12655,7 +12834,7 @@
       <c r="G75" s="55"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="247"/>
+      <c r="C76" s="249"/>
       <c r="D76" s="60" t="s">
         <v>95</v>
       </c>
@@ -12668,7 +12847,7 @@
       <c r="G76" s="63"/>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="247"/>
+      <c r="C77" s="249"/>
       <c r="D77" s="65" t="s">
         <v>116</v>
       </c>
@@ -12679,7 +12858,7 @@
       <c r="G77" s="68"/>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="247"/>
+      <c r="C78" s="249"/>
       <c r="D78" s="56" t="s">
         <v>119</v>
       </c>
@@ -12689,7 +12868,7 @@
       <c r="G78" s="55"/>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="247"/>
+      <c r="C79" s="249"/>
       <c r="D79" s="60" t="s">
         <v>121</v>
       </c>
@@ -12700,7 +12879,7 @@
       <c r="G79" s="63"/>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="247"/>
+      <c r="C80" s="249"/>
       <c r="D80" s="65" t="s">
         <v>116</v>
       </c>
@@ -12711,7 +12890,7 @@
       <c r="G80" s="68"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="247"/>
+      <c r="C81" s="249"/>
       <c r="D81" s="56" t="s">
         <v>126</v>
       </c>
@@ -12724,7 +12903,7 @@
       <c r="G81" s="55"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="247"/>
+      <c r="C82" s="249"/>
       <c r="D82" s="56" t="s">
         <v>119</v>
       </c>
@@ -12737,7 +12916,7 @@
       <c r="G82" s="55"/>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="248"/>
+      <c r="C83" s="250"/>
       <c r="D83" s="60" t="s">
         <v>110</v>
       </c>
@@ -12831,12 +13010,12 @@
       <c r="V8" s="75"/>
     </row>
     <row r="9" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D9" s="257" t="s">
+      <c r="D9" s="264" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="258"/>
-      <c r="F9" s="258"/>
-      <c r="G9" s="259"/>
+      <c r="E9" s="265"/>
+      <c r="F9" s="265"/>
+      <c r="G9" s="266"/>
       <c r="V9" s="75"/>
     </row>
     <row r="10" spans="4:23" x14ac:dyDescent="0.25">
@@ -13010,7 +13189,7 @@
       </c>
     </row>
     <row r="17" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D17" s="233" t="s">
+      <c r="D17" s="235" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="69" t="s">
@@ -13034,7 +13213,7 @@
       <c r="V17" s="75"/>
     </row>
     <row r="18" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D18" s="233"/>
+      <c r="D18" s="235"/>
       <c r="E18" s="69" t="s">
         <v>140</v>
       </c>
@@ -13056,7 +13235,7 @@
       <c r="V18" s="75"/>
     </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D19" s="233"/>
+      <c r="D19" s="235"/>
       <c r="E19" s="69" t="s">
         <v>141</v>
       </c>
@@ -13182,7 +13361,7 @@
       <c r="D31" s="96"/>
     </row>
     <row r="32" spans="3:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="264" t="s">
+      <c r="C32" s="267" t="s">
         <v>207</v>
       </c>
       <c r="D32" s="85" t="s">
@@ -13193,7 +13372,7 @@
       <c r="G32" s="87"/>
     </row>
     <row r="33" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C33" s="265"/>
+      <c r="C33" s="268"/>
       <c r="D33" s="89" t="s">
         <v>180</v>
       </c>
@@ -13204,7 +13383,7 @@
       <c r="G33" s="87"/>
     </row>
     <row r="34" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C34" s="265"/>
+      <c r="C34" s="268"/>
       <c r="D34" s="90" t="s">
         <v>181</v>
       </c>
@@ -13214,7 +13393,7 @@
       <c r="G34" s="88"/>
     </row>
     <row r="35" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C35" s="265"/>
+      <c r="C35" s="268"/>
       <c r="D35" s="90" t="s">
         <v>183</v>
       </c>
@@ -13226,7 +13405,7 @@
       </c>
     </row>
     <row r="36" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C36" s="265"/>
+      <c r="C36" s="268"/>
       <c r="D36" s="91" t="s">
         <v>185</v>
       </c>
@@ -13241,7 +13420,7 @@
       </c>
     </row>
     <row r="37" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C37" s="265"/>
+      <c r="C37" s="268"/>
       <c r="D37" s="94" t="s">
         <v>187</v>
       </c>
@@ -13254,7 +13433,7 @@
       </c>
     </row>
     <row r="38" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C38" s="265"/>
+      <c r="C38" s="268"/>
       <c r="D38" s="89" t="s">
         <v>193</v>
       </c>
@@ -13279,7 +13458,7 @@
       </c>
     </row>
     <row r="39" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C39" s="265"/>
+      <c r="C39" s="268"/>
       <c r="D39" s="90" t="s">
         <v>194</v>
       </c>
@@ -13301,7 +13480,7 @@
       </c>
     </row>
     <row r="40" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C40" s="265"/>
+      <c r="C40" s="268"/>
       <c r="D40" s="90" t="s">
         <v>195</v>
       </c>
@@ -13342,7 +13521,7 @@
       </c>
     </row>
     <row r="41" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C41" s="265"/>
+      <c r="C41" s="268"/>
       <c r="D41" s="91" t="s">
         <v>196</v>
       </c>
@@ -13383,7 +13562,7 @@
       </c>
     </row>
     <row r="42" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C42" s="265"/>
+      <c r="C42" s="268"/>
       <c r="D42" s="80" t="s">
         <v>197</v>
       </c>
@@ -13416,15 +13595,15 @@
       </c>
     </row>
     <row r="43" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C43" s="265"/>
+      <c r="C43" s="268"/>
       <c r="D43" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E43" s="260" t="s">
+      <c r="E43" s="259" t="s">
         <v>200</v>
       </c>
-      <c r="F43" s="260"/>
-      <c r="G43" s="261"/>
+      <c r="F43" s="259"/>
+      <c r="G43" s="260"/>
       <c r="AA43" s="44">
         <v>13</v>
       </c>
@@ -13453,13 +13632,13 @@
       </c>
     </row>
     <row r="44" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C44" s="266"/>
+      <c r="C44" s="269"/>
       <c r="D44" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="E44" s="262"/>
-      <c r="F44" s="262"/>
-      <c r="G44" s="263"/>
+      <c r="E44" s="261"/>
+      <c r="F44" s="261"/>
+      <c r="G44" s="262"/>
       <c r="AA44" s="44">
         <v>14</v>
       </c>
@@ -13488,7 +13667,7 @@
       </c>
     </row>
     <row r="45" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C45" s="272" t="s">
+      <c r="C45" s="263" t="s">
         <v>216</v>
       </c>
       <c r="D45" s="94" t="s">
@@ -13525,7 +13704,7 @@
       </c>
     </row>
     <row r="46" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C46" s="272"/>
+      <c r="C46" s="263"/>
       <c r="D46" s="89" t="s">
         <v>180</v>
       </c>
@@ -13562,7 +13741,7 @@
       </c>
     </row>
     <row r="47" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C47" s="272"/>
+      <c r="C47" s="263"/>
       <c r="D47" s="90" t="s">
         <v>181</v>
       </c>
@@ -13598,7 +13777,7 @@
       </c>
     </row>
     <row r="48" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C48" s="272"/>
+      <c r="C48" s="263"/>
       <c r="D48" s="90" t="s">
         <v>183</v>
       </c>
@@ -13636,7 +13815,7 @@
       </c>
     </row>
     <row r="49" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C49" s="272"/>
+      <c r="C49" s="263"/>
       <c r="D49" s="90" t="s">
         <v>185</v>
       </c>
@@ -13677,7 +13856,7 @@
       </c>
     </row>
     <row r="50" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C50" s="272"/>
+      <c r="C50" s="263"/>
       <c r="D50" s="93" t="s">
         <v>187</v>
       </c>
@@ -13710,7 +13889,7 @@
       </c>
     </row>
     <row r="51" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C51" s="272"/>
+      <c r="C51" s="263"/>
       <c r="D51" s="90" t="s">
         <v>212</v>
       </c>
@@ -13751,7 +13930,7 @@
       </c>
     </row>
     <row r="52" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C52" s="272"/>
+      <c r="C52" s="263"/>
       <c r="D52" s="93" t="s">
         <v>197</v>
       </c>
@@ -13784,15 +13963,15 @@
       </c>
     </row>
     <row r="53" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C53" s="272"/>
+      <c r="C53" s="263"/>
       <c r="D53" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="260" t="s">
+      <c r="E53" s="259" t="s">
         <v>200</v>
       </c>
-      <c r="F53" s="260"/>
-      <c r="G53" s="261"/>
+      <c r="F53" s="259"/>
+      <c r="G53" s="260"/>
       <c r="AA53" s="44">
         <v>23</v>
       </c>
@@ -13821,13 +14000,13 @@
       </c>
     </row>
     <row r="54" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C54" s="272"/>
+      <c r="C54" s="263"/>
       <c r="D54" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E54" s="262"/>
-      <c r="F54" s="262"/>
-      <c r="G54" s="263"/>
+      <c r="E54" s="261"/>
+      <c r="F54" s="261"/>
+      <c r="G54" s="262"/>
       <c r="AA54" s="44">
         <v>24</v>
       </c>
@@ -13856,7 +14035,7 @@
       </c>
     </row>
     <row r="55" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C55" s="272"/>
+      <c r="C55" s="263"/>
       <c r="D55" s="94" t="s">
         <v>186</v>
       </c>
@@ -13891,7 +14070,7 @@
       </c>
     </row>
     <row r="56" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C56" s="272"/>
+      <c r="C56" s="263"/>
       <c r="D56" s="89" t="s">
         <v>180</v>
       </c>
@@ -13928,7 +14107,7 @@
       </c>
     </row>
     <row r="57" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C57" s="272"/>
+      <c r="C57" s="263"/>
       <c r="D57" s="90" t="s">
         <v>181</v>
       </c>
@@ -13964,7 +14143,7 @@
       </c>
     </row>
     <row r="58" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C58" s="272"/>
+      <c r="C58" s="263"/>
       <c r="D58" s="90" t="s">
         <v>183</v>
       </c>
@@ -14002,7 +14181,7 @@
       </c>
     </row>
     <row r="59" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C59" s="272"/>
+      <c r="C59" s="263"/>
       <c r="D59" s="91" t="s">
         <v>185</v>
       </c>
@@ -14043,7 +14222,7 @@
       </c>
     </row>
     <row r="60" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C60" s="272"/>
+      <c r="C60" s="263"/>
       <c r="D60" s="94" t="s">
         <v>187</v>
       </c>
@@ -14078,7 +14257,7 @@
       </c>
     </row>
     <row r="61" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C61" s="272"/>
+      <c r="C61" s="263"/>
       <c r="D61" s="89" t="s">
         <v>212</v>
       </c>
@@ -14119,7 +14298,7 @@
       </c>
     </row>
     <row r="62" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C62" s="272"/>
+      <c r="C62" s="263"/>
       <c r="D62" s="93" t="s">
         <v>197</v>
       </c>
@@ -14152,15 +14331,15 @@
       </c>
     </row>
     <row r="63" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C63" s="272"/>
+      <c r="C63" s="263"/>
       <c r="D63" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E63" s="260" t="s">
+      <c r="E63" s="259" t="s">
         <v>200</v>
       </c>
-      <c r="F63" s="260"/>
-      <c r="G63" s="261"/>
+      <c r="F63" s="259"/>
+      <c r="G63" s="260"/>
       <c r="AA63" s="44">
         <v>33</v>
       </c>
@@ -14189,13 +14368,13 @@
       </c>
     </row>
     <row r="64" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C64" s="272"/>
+      <c r="C64" s="263"/>
       <c r="D64" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="262"/>
-      <c r="F64" s="262"/>
-      <c r="G64" s="263"/>
+      <c r="E64" s="261"/>
+      <c r="F64" s="261"/>
+      <c r="G64" s="262"/>
       <c r="AA64" s="44">
         <v>34</v>
       </c>
@@ -14347,22 +14526,22 @@
       </c>
     </row>
     <row r="69" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C69" s="264" t="s">
+      <c r="C69" s="267" t="s">
         <v>160</v>
       </c>
-      <c r="D69" s="270" t="s">
+      <c r="D69" s="273" t="s">
         <v>161</v>
       </c>
-      <c r="E69" s="270"/>
-      <c r="F69" s="270" t="s">
+      <c r="E69" s="273"/>
+      <c r="F69" s="273" t="s">
         <v>133</v>
       </c>
-      <c r="G69" s="271"/>
-      <c r="I69" s="267" t="s">
+      <c r="G69" s="274"/>
+      <c r="I69" s="270" t="s">
         <v>223</v>
       </c>
-      <c r="J69" s="268"/>
-      <c r="K69" s="269"/>
+      <c r="J69" s="271"/>
+      <c r="K69" s="272"/>
       <c r="AA69" s="44">
         <v>39</v>
       </c>
@@ -14391,7 +14570,7 @@
       </c>
     </row>
     <row r="70" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C70" s="265"/>
+      <c r="C70" s="268"/>
       <c r="D70" s="15" t="s">
         <v>162</v>
       </c>
@@ -14799,11 +14978,11 @@
         <f t="shared" si="10"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="I77" s="267" t="s">
+      <c r="I77" s="270" t="s">
         <v>222</v>
       </c>
-      <c r="J77" s="268"/>
-      <c r="K77" s="269"/>
+      <c r="J77" s="271"/>
+      <c r="K77" s="272"/>
       <c r="AA77" s="44">
         <v>47</v>
       </c>
@@ -15323,7 +15502,7 @@
       </c>
     </row>
     <row r="90" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C90" s="253" t="s">
+      <c r="C90" s="255" t="s">
         <v>230</v>
       </c>
       <c r="D90" s="86" t="s">
@@ -15376,7 +15555,7 @@
       </c>
     </row>
     <row r="91" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C91" s="254"/>
+      <c r="C91" s="256"/>
       <c r="D91" s="44" t="s">
         <v>232</v>
       </c>
@@ -15427,7 +15606,7 @@
       </c>
     </row>
     <row r="92" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C92" s="254" t="s">
+      <c r="C92" s="256" t="s">
         <v>233</v>
       </c>
       <c r="D92" s="44" t="s">
@@ -15480,7 +15659,7 @@
       </c>
     </row>
     <row r="93" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C93" s="254"/>
+      <c r="C93" s="256"/>
       <c r="D93" s="44" t="s">
         <v>236</v>
       </c>
@@ -15531,7 +15710,7 @@
       </c>
     </row>
     <row r="94" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C94" s="255" t="s">
+      <c r="C94" s="257" t="s">
         <v>234</v>
       </c>
       <c r="D94" s="44" t="s">
@@ -15584,7 +15763,7 @@
       </c>
     </row>
     <row r="95" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C95" s="256"/>
+      <c r="C95" s="258"/>
       <c r="D95" s="81" t="s">
         <v>238</v>
       </c>
@@ -15952,7 +16131,7 @@
       </c>
     </row>
     <row r="126" spans="3:24" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C126" s="253" t="s">
+      <c r="C126" s="255" t="s">
         <v>230</v>
       </c>
       <c r="D126" s="86" t="s">
@@ -15979,7 +16158,7 @@
       </c>
     </row>
     <row r="127" spans="3:24" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C127" s="254"/>
+      <c r="C127" s="256"/>
       <c r="D127" s="44" t="s">
         <v>232</v>
       </c>
@@ -16004,7 +16183,7 @@
       </c>
     </row>
     <row r="128" spans="3:24" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C128" s="254" t="s">
+      <c r="C128" s="256" t="s">
         <v>233</v>
       </c>
       <c r="D128" s="44" t="s">
@@ -16031,7 +16210,7 @@
       </c>
     </row>
     <row r="129" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C129" s="254"/>
+      <c r="C129" s="256"/>
       <c r="D129" s="44" t="s">
         <v>236</v>
       </c>
@@ -16056,7 +16235,7 @@
       </c>
     </row>
     <row r="130" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C130" s="255" t="s">
+      <c r="C130" s="257" t="s">
         <v>234</v>
       </c>
       <c r="D130" s="44" t="s">
@@ -16083,7 +16262,7 @@
       </c>
     </row>
     <row r="131" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C131" s="256"/>
+      <c r="C131" s="258"/>
       <c r="D131" s="81" t="s">
         <v>238</v>
       </c>
@@ -16318,7 +16497,7 @@
       </c>
     </row>
     <row r="163" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C163" s="253" t="s">
+      <c r="C163" s="255" t="s">
         <v>230</v>
       </c>
       <c r="D163" s="86" t="s">
@@ -16345,7 +16524,7 @@
       </c>
     </row>
     <row r="164" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C164" s="254"/>
+      <c r="C164" s="256"/>
       <c r="D164" s="44" t="s">
         <v>232</v>
       </c>
@@ -16370,7 +16549,7 @@
       </c>
     </row>
     <row r="165" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C165" s="254" t="s">
+      <c r="C165" s="256" t="s">
         <v>233</v>
       </c>
       <c r="D165" s="44" t="s">
@@ -16397,7 +16576,7 @@
       </c>
     </row>
     <row r="166" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C166" s="254"/>
+      <c r="C166" s="256"/>
       <c r="D166" s="44" t="s">
         <v>236</v>
       </c>
@@ -16422,7 +16601,7 @@
       </c>
     </row>
     <row r="167" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C167" s="255" t="s">
+      <c r="C167" s="257" t="s">
         <v>234</v>
       </c>
       <c r="D167" s="44" t="s">
@@ -16449,7 +16628,7 @@
       </c>
     </row>
     <row r="168" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C168" s="256"/>
+      <c r="C168" s="258"/>
       <c r="D168" s="81" t="s">
         <v>238</v>
       </c>
@@ -16633,12 +16812,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="E53:G54"/>
-    <mergeCell ref="E63:G64"/>
-    <mergeCell ref="C45:C64"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="C130:C131"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="E43:G44"/>
@@ -16648,12 +16827,12 @@
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="F69:G69"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="E53:G54"/>
+    <mergeCell ref="E63:G64"/>
+    <mergeCell ref="C45:C64"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16703,27 +16882,27 @@
       <c r="L4" s="81"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="267" t="s">
+      <c r="C5" s="270" t="s">
         <v>314</v>
       </c>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
-      <c r="G5" s="268"/>
-      <c r="H5" s="269"/>
+      <c r="D5" s="271"/>
+      <c r="E5" s="271"/>
+      <c r="F5" s="271"/>
+      <c r="G5" s="271"/>
+      <c r="H5" s="272"/>
       <c r="I5" s="171" t="s">
         <v>315</v>
       </c>
-      <c r="J5" s="267" t="s">
+      <c r="J5" s="270" t="s">
         <v>316</v>
       </c>
-      <c r="K5" s="268"/>
-      <c r="L5" s="268"/>
-      <c r="M5" s="273" t="s">
+      <c r="K5" s="271"/>
+      <c r="L5" s="271"/>
+      <c r="M5" s="275" t="s">
         <v>322</v>
       </c>
-      <c r="N5" s="270"/>
-      <c r="O5" s="271"/>
+      <c r="N5" s="273"/>
+      <c r="O5" s="274"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="168" t="s">
@@ -16929,26 +17108,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="D2" s="274" t="s">
+      <c r="D2" s="276" t="s">
         <v>356</v>
       </c>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="276"/>
-      <c r="L2" s="274" t="s">
+      <c r="E2" s="277"/>
+      <c r="F2" s="277"/>
+      <c r="G2" s="277"/>
+      <c r="H2" s="277"/>
+      <c r="I2" s="277"/>
+      <c r="J2" s="277"/>
+      <c r="K2" s="278"/>
+      <c r="L2" s="276" t="s">
         <v>357</v>
       </c>
-      <c r="M2" s="275"/>
-      <c r="N2" s="275"/>
-      <c r="O2" s="275"/>
-      <c r="P2" s="275"/>
-      <c r="Q2" s="275"/>
-      <c r="R2" s="275"/>
-      <c r="S2" s="276"/>
+      <c r="M2" s="277"/>
+      <c r="N2" s="277"/>
+      <c r="O2" s="277"/>
+      <c r="P2" s="277"/>
+      <c r="Q2" s="277"/>
+      <c r="R2" s="277"/>
+      <c r="S2" s="278"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B3" s="204" t="s">
@@ -17416,7 +17595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -17910,14 +18089,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E5" s="277" t="s">
+      <c r="E5" s="279" t="s">
         <v>366</v>
       </c>
-      <c r="F5" s="278"/>
-      <c r="G5" s="279" t="s">
+      <c r="F5" s="280"/>
+      <c r="G5" s="281" t="s">
         <v>367</v>
       </c>
-      <c r="H5" s="280"/>
+      <c r="H5" s="282"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="217" t="s">

</xml_diff>

<commit_message>
Se obtienen figuras finales
</commit_message>
<xml_diff>
--- a/Validacion/RW-A20-P10-S38/Documentation/Documentacion RW-A20-P10-S38.xlsx
+++ b/Validacion/RW-A20-P10-S38/Documentation/Documentacion RW-A20-P10-S38.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryj\Documents\GitHub\Ejemplos\Validacion\RW-A20-P10-S38\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4E4A7E-46FD-4EFB-A3D4-74478D5D3DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8572FE90-56F9-4517-87FD-C465B8F1239A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="383">
   <si>
     <t>m</t>
   </si>
@@ -1479,6 +1479,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>1 ELEMENTO PARA EL LARGO TOTAL DE ROTULA PLASTICA</t>
+  </si>
+  <si>
+    <t>2 ELEMENTOS PARA EL LARGO TOTAL DE ROTULA PLASTICA</t>
+  </si>
+  <si>
+    <t>ENERGIA DE FRACTURA</t>
   </si>
 </sst>
 </file>
@@ -2174,7 +2183,7 @@
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="284">
+  <cellXfs count="295">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2691,6 +2700,12 @@
     <xf numFmtId="166" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2838,7 +2853,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -7221,16 +7251,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>520651</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>183466</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>288245</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>150981</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>560660</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>95736</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7253,8 +7283,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4787851" y="5000625"/>
-          <a:ext cx="3971929" cy="4608681"/>
+          <a:off x="5669866" y="5486400"/>
+          <a:ext cx="3968119" cy="4610586"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7265,16 +7295,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>372828</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>626193</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>250600</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>60048</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>180115</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>35283</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7297,8 +7327,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13517328" y="4819650"/>
-          <a:ext cx="4417387" cy="4694913"/>
+          <a:off x="14751768" y="5311140"/>
+          <a:ext cx="4421197" cy="4725393"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7956,7 +7986,7 @@
   <dimension ref="H1:V73"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:N32"/>
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7979,20 +8009,20 @@
   <sheetData>
     <row r="1" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="237" t="s">
+      <c r="J2" s="239" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="238"/>
-      <c r="L2" s="238"/>
-      <c r="M2" s="238"/>
-      <c r="N2" s="239"/>
-      <c r="Q2" s="237" t="s">
+      <c r="K2" s="240"/>
+      <c r="L2" s="240"/>
+      <c r="M2" s="240"/>
+      <c r="N2" s="241"/>
+      <c r="Q2" s="239" t="s">
         <v>336</v>
       </c>
-      <c r="R2" s="238"/>
-      <c r="S2" s="238"/>
-      <c r="T2" s="238"/>
-      <c r="U2" s="239"/>
+      <c r="R2" s="240"/>
+      <c r="S2" s="240"/>
+      <c r="T2" s="240"/>
+      <c r="U2" s="241"/>
     </row>
     <row r="3" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J3" s="11"/>
@@ -8004,7 +8034,7 @@
       <c r="N3" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="Q3" s="243" t="s">
+      <c r="Q3" s="245" t="s">
         <v>3</v>
       </c>
       <c r="R3" s="18" t="s">
@@ -8031,7 +8061,7 @@
         <f>M4/25.4</f>
         <v>96.000000000000014</v>
       </c>
-      <c r="Q4" s="244"/>
+      <c r="Q4" s="246"/>
       <c r="R4" s="1"/>
       <c r="S4" s="166"/>
       <c r="T4" s="2"/>
@@ -8051,7 +8081,7 @@
         <f>M5/25.4</f>
         <v>48.031496062992126</v>
       </c>
-      <c r="Q5" s="244"/>
+      <c r="Q5" s="246"/>
       <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
@@ -8073,7 +8103,7 @@
         <f t="shared" ref="N6:N7" si="0">M6/25.4</f>
         <v>6.0000000000000009</v>
       </c>
-      <c r="Q6" s="244"/>
+      <c r="Q6" s="246"/>
       <c r="R6" s="23" t="s">
         <v>6</v>
       </c>
@@ -8095,7 +8125,7 @@
         <f t="shared" si="0"/>
         <v>12.000000000000002</v>
       </c>
-      <c r="Q7" s="244"/>
+      <c r="Q7" s="246"/>
       <c r="R7" s="23" t="s">
         <v>7</v>
       </c>
@@ -8124,7 +8154,7 @@
         <f>M8/25.4</f>
         <v>9</v>
       </c>
-      <c r="Q8" s="244"/>
+      <c r="Q8" s="246"/>
       <c r="R8" s="23" t="s">
         <v>10</v>
       </c>
@@ -8149,7 +8179,7 @@
       <c r="N9" s="200" t="s">
         <v>353</v>
       </c>
-      <c r="Q9" s="244"/>
+      <c r="Q9" s="246"/>
       <c r="R9" s="3" t="s">
         <v>11</v>
       </c>
@@ -8162,7 +8192,7 @@
       <c r="U9" s="29"/>
     </row>
     <row r="10" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q10" s="244"/>
+      <c r="Q10" s="246"/>
       <c r="R10" s="6" t="s">
         <v>13</v>
       </c>
@@ -8171,14 +8201,14 @@
       <c r="U10" s="30"/>
     </row>
     <row r="11" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="240" t="s">
+      <c r="J11" s="242" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="241"/>
-      <c r="L11" s="241"/>
-      <c r="M11" s="241"/>
-      <c r="N11" s="242"/>
-      <c r="Q11" s="244"/>
+      <c r="K11" s="243"/>
+      <c r="L11" s="243"/>
+      <c r="M11" s="243"/>
+      <c r="N11" s="244"/>
+      <c r="Q11" s="246"/>
       <c r="R11" s="23" t="s">
         <v>6</v>
       </c>
@@ -8202,7 +8232,7 @@
       <c r="N12" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="Q12" s="244"/>
+      <c r="Q12" s="246"/>
       <c r="R12" s="23" t="s">
         <v>7</v>
       </c>
@@ -8234,7 +8264,7 @@
         <f>M13/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="244"/>
+      <c r="Q13" s="246"/>
       <c r="R13" s="23" t="s">
         <v>10</v>
       </c>
@@ -8262,7 +8292,7 @@
         <f t="shared" ref="N14:N32" si="2">M14/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="244"/>
+      <c r="Q14" s="246"/>
       <c r="R14" s="3" t="s">
         <v>11</v>
       </c>
@@ -8296,7 +8326,7 @@
         <f>M15-$M$15/2</f>
         <v>157.845</v>
       </c>
-      <c r="Q15" s="244"/>
+      <c r="Q15" s="246"/>
       <c r="R15" s="6" t="s">
         <v>16</v>
       </c>
@@ -8323,10 +8353,10 @@
         <v>12.428740157480316</v>
       </c>
       <c r="O16" s="226">
-        <f t="shared" ref="O16:O26" si="3">M16-$M$15/2</f>
+        <f>M16-$M$15/2</f>
         <v>157.845</v>
       </c>
-      <c r="Q16" s="244"/>
+      <c r="Q16" s="246"/>
       <c r="R16" s="23" t="s">
         <v>6</v>
       </c>
@@ -8356,7 +8386,7 @@
         <f>M17-$M$15/2</f>
         <v>473.52499999999998</v>
       </c>
-      <c r="Q17" s="244"/>
+      <c r="Q17" s="246"/>
       <c r="R17" s="23" t="s">
         <v>7</v>
       </c>
@@ -8389,10 +8419,10 @@
         <v>24.85708661417323</v>
       </c>
       <c r="O18" s="226">
-        <f t="shared" si="3"/>
+        <f>M18-$M$15/2</f>
         <v>473.52499999999998</v>
       </c>
-      <c r="Q18" s="244"/>
+      <c r="Q18" s="246"/>
       <c r="R18" s="23" t="s">
         <v>10</v>
       </c>
@@ -8421,10 +8451,10 @@
         <v>37.285826771653547</v>
       </c>
       <c r="O19" s="226">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="O19:O22" si="3">M19-$M$15/2</f>
         <v>789.21499999999992</v>
       </c>
-      <c r="Q19" s="244"/>
+      <c r="Q19" s="246"/>
       <c r="R19" s="3" t="s">
         <v>11</v>
       </c>
@@ -8459,7 +8489,7 @@
         <f t="shared" si="3"/>
         <v>789.21499999999992</v>
       </c>
-      <c r="Q20" s="244"/>
+      <c r="Q20" s="246"/>
       <c r="R20" s="32" t="s">
         <v>19</v>
       </c>
@@ -8492,10 +8522,10 @@
         <v>49.714173228346461</v>
       </c>
       <c r="O21" s="226">
-        <f t="shared" si="3"/>
+        <f>M21-$M$15/2</f>
         <v>1104.895</v>
       </c>
-      <c r="Q21" s="244"/>
+      <c r="Q21" s="246"/>
       <c r="R21" s="32" t="s">
         <v>21</v>
       </c>
@@ -8529,7 +8559,7 @@
         <f t="shared" si="3"/>
         <v>1104.895</v>
       </c>
-      <c r="Q22" s="244"/>
+      <c r="Q22" s="246"/>
       <c r="R22" s="32" t="s">
         <v>24</v>
       </c>
@@ -8560,10 +8590,10 @@
         <v>62.14291338582678</v>
       </c>
       <c r="O23" s="226">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="O23:O28" si="4">M23-$M$15/2</f>
         <v>1420.585</v>
       </c>
-      <c r="Q23" s="245"/>
+      <c r="Q23" s="247"/>
       <c r="R23" s="2"/>
       <c r="S23" s="8" t="s">
         <v>26</v>
@@ -8592,10 +8622,10 @@
         <v>62.14291338582678</v>
       </c>
       <c r="O24" s="226">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1420.585</v>
       </c>
-      <c r="Q24" s="246" t="s">
+      <c r="Q24" s="248" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -8626,10 +8656,10 @@
         <v>74.57125984251968</v>
       </c>
       <c r="O25" s="226">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1736.2649999999999</v>
       </c>
-      <c r="Q25" s="244"/>
+      <c r="Q25" s="246"/>
       <c r="R25" s="6" t="s">
         <v>29</v>
       </c>
@@ -8656,10 +8686,10 @@
         <v>74.57125984251968</v>
       </c>
       <c r="O26" s="226">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1736.2649999999999</v>
       </c>
-      <c r="Q26" s="244"/>
+      <c r="Q26" s="246"/>
       <c r="R26" s="23" t="s">
         <v>30</v>
       </c>
@@ -8692,10 +8722,10 @@
         <v>87.000000000000014</v>
       </c>
       <c r="O27" s="226">
-        <f>M27-$M$15/2</f>
+        <f t="shared" si="4"/>
         <v>2051.9550000000004</v>
       </c>
-      <c r="Q27" s="244"/>
+      <c r="Q27" s="246"/>
       <c r="R27" s="23" t="s">
         <v>32</v>
       </c>
@@ -8726,10 +8756,10 @@
         <v>87.000000000000014</v>
       </c>
       <c r="O28" s="226">
-        <f>M28-$M$15/2</f>
+        <f t="shared" si="4"/>
         <v>2051.9550000000004</v>
       </c>
-      <c r="Q28" s="244"/>
+      <c r="Q28" s="246"/>
       <c r="R28" s="23" t="s">
         <v>19</v>
       </c>
@@ -8766,7 +8796,7 @@
         <f>M29-228.6/2</f>
         <v>2324.1</v>
       </c>
-      <c r="Q29" s="244"/>
+      <c r="Q29" s="246"/>
       <c r="R29" s="23" t="s">
         <v>34</v>
       </c>
@@ -8798,7 +8828,7 @@
         <v>96.000000000000014</v>
       </c>
       <c r="O30" s="178"/>
-      <c r="Q30" s="244"/>
+      <c r="Q30" s="246"/>
       <c r="R30" s="23" t="s">
         <v>36</v>
       </c>
@@ -8830,7 +8860,7 @@
         <v>105</v>
       </c>
       <c r="O31" s="178"/>
-      <c r="Q31" s="244"/>
+      <c r="Q31" s="246"/>
       <c r="R31" s="6" t="s">
         <v>37</v>
       </c>
@@ -8857,7 +8887,7 @@
         <v>105</v>
       </c>
       <c r="O32" s="178"/>
-      <c r="Q32" s="244"/>
+      <c r="Q32" s="246"/>
       <c r="R32" s="23" t="s">
         <v>38</v>
       </c>
@@ -8872,7 +8902,7 @@
       </c>
     </row>
     <row r="33" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q33" s="244"/>
+      <c r="Q33" s="246"/>
       <c r="R33" s="23" t="s">
         <v>40</v>
       </c>
@@ -8885,7 +8915,7 @@
       <c r="U33" s="25"/>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q34" s="244"/>
+      <c r="Q34" s="246"/>
       <c r="R34" s="23" t="s">
         <v>42</v>
       </c>
@@ -8901,7 +8931,7 @@
       </c>
     </row>
     <row r="35" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q35" s="244"/>
+      <c r="Q35" s="246"/>
       <c r="R35" s="23" t="s">
         <v>34</v>
       </c>
@@ -8914,7 +8944,7 @@
       <c r="U35" s="25"/>
     </row>
     <row r="36" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q36" s="244"/>
+      <c r="Q36" s="246"/>
       <c r="R36" s="23" t="s">
         <v>36</v>
       </c>
@@ -8928,7 +8958,7 @@
       <c r="U36" s="190"/>
     </row>
     <row r="37" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q37" s="244"/>
+      <c r="Q37" s="246"/>
       <c r="R37" s="6" t="s">
         <v>44</v>
       </c>
@@ -8937,7 +8967,7 @@
       <c r="U37" s="30"/>
     </row>
     <row r="38" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q38" s="244"/>
+      <c r="Q38" s="246"/>
       <c r="R38" s="23" t="s">
         <v>45</v>
       </c>
@@ -8953,7 +8983,7 @@
       </c>
     </row>
     <row r="39" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q39" s="244"/>
+      <c r="Q39" s="246"/>
       <c r="R39" s="23" t="s">
         <v>46</v>
       </c>
@@ -8966,7 +8996,7 @@
       <c r="U39" s="25"/>
     </row>
     <row r="40" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="244"/>
+      <c r="Q40" s="246"/>
       <c r="R40" s="23" t="s">
         <v>34</v>
       </c>
@@ -8981,7 +9011,7 @@
       </c>
     </row>
     <row r="41" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="245"/>
+      <c r="Q41" s="247"/>
       <c r="R41" s="23" t="s">
         <v>36</v>
       </c>
@@ -8994,7 +9024,7 @@
       <c r="U41" s="22"/>
     </row>
     <row r="42" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q42" s="247" t="s">
+      <c r="Q42" s="249" t="s">
         <v>50</v>
       </c>
       <c r="R42" s="6" t="s">
@@ -9007,7 +9037,7 @@
       <c r="U42" s="30"/>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q43" s="235"/>
+      <c r="Q43" s="237"/>
       <c r="R43" s="6" t="s">
         <v>52</v>
       </c>
@@ -9016,7 +9046,7 @@
       <c r="U43" s="30"/>
     </row>
     <row r="44" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q44" s="235"/>
+      <c r="Q44" s="237"/>
       <c r="R44" s="23" t="s">
         <v>53</v>
       </c>
@@ -9027,7 +9057,7 @@
       <c r="U44" s="25"/>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q45" s="235"/>
+      <c r="Q45" s="237"/>
       <c r="R45" s="23" t="s">
         <v>54</v>
       </c>
@@ -9042,7 +9072,7 @@
       </c>
     </row>
     <row r="46" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q46" s="235"/>
+      <c r="Q46" s="237"/>
       <c r="R46" s="23" t="s">
         <v>57</v>
       </c>
@@ -9057,7 +9087,7 @@
       </c>
     </row>
     <row r="47" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q47" s="235"/>
+      <c r="Q47" s="237"/>
       <c r="R47" s="23" t="s">
         <v>59</v>
       </c>
@@ -9073,7 +9103,7 @@
       </c>
     </row>
     <row r="48" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q48" s="235"/>
+      <c r="Q48" s="237"/>
       <c r="R48" s="23"/>
       <c r="S48" s="26" t="s">
         <v>306</v>
@@ -9085,7 +9115,7 @@
       <c r="U48" s="25"/>
     </row>
     <row r="49" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q49" s="235"/>
+      <c r="Q49" s="237"/>
       <c r="R49" s="23" t="s">
         <v>61</v>
       </c>
@@ -9099,7 +9129,7 @@
       <c r="U49" s="25"/>
     </row>
     <row r="50" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q50" s="235"/>
+      <c r="Q50" s="237"/>
       <c r="R50" s="6" t="s">
         <v>62</v>
       </c>
@@ -9111,7 +9141,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="Q51" s="235"/>
+      <c r="Q51" s="237"/>
       <c r="R51" s="23" t="s">
         <v>63</v>
       </c>
@@ -9126,7 +9156,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="N52" s="144"/>
-      <c r="Q52" s="235"/>
+      <c r="Q52" s="237"/>
       <c r="R52" s="23" t="s">
         <v>54</v>
       </c>
@@ -9144,7 +9174,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
-      <c r="Q53" s="235"/>
+      <c r="Q53" s="237"/>
       <c r="R53" s="23" t="s">
         <v>64</v>
       </c>
@@ -9160,7 +9190,7 @@
       </c>
     </row>
     <row r="54" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q54" s="235"/>
+      <c r="Q54" s="237"/>
       <c r="R54" s="23" t="s">
         <v>66</v>
       </c>
@@ -9176,7 +9206,7 @@
       </c>
     </row>
     <row r="55" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q55" s="235"/>
+      <c r="Q55" s="237"/>
       <c r="R55" s="23" t="s">
         <v>61</v>
       </c>
@@ -9190,7 +9220,7 @@
       <c r="U55" s="25"/>
     </row>
     <row r="56" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q56" s="235"/>
+      <c r="Q56" s="237"/>
       <c r="R56" s="6" t="s">
         <v>69</v>
       </c>
@@ -9199,7 +9229,7 @@
       <c r="U56" s="30"/>
     </row>
     <row r="57" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q57" s="235"/>
+      <c r="Q57" s="237"/>
       <c r="R57" s="23" t="s">
         <v>70</v>
       </c>
@@ -9210,7 +9240,7 @@
       <c r="U57" s="25"/>
     </row>
     <row r="58" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q58" s="235"/>
+      <c r="Q58" s="237"/>
       <c r="R58" s="23" t="s">
         <v>54</v>
       </c>
@@ -9226,7 +9256,7 @@
       <c r="V58" s="27"/>
     </row>
     <row r="59" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q59" s="235"/>
+      <c r="Q59" s="237"/>
       <c r="R59" s="23" t="s">
         <v>57</v>
       </c>
@@ -9241,7 +9271,7 @@
       </c>
     </row>
     <row r="60" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q60" s="235"/>
+      <c r="Q60" s="237"/>
       <c r="R60" s="23" t="s">
         <v>71</v>
       </c>
@@ -9254,7 +9284,7 @@
       <c r="U60" s="25"/>
     </row>
     <row r="61" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q61" s="235"/>
+      <c r="Q61" s="237"/>
       <c r="R61" s="23" t="s">
         <v>59</v>
       </c>
@@ -9271,7 +9301,7 @@
       <c r="V61" s="37"/>
     </row>
     <row r="62" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q62" s="235"/>
+      <c r="Q62" s="237"/>
       <c r="R62" s="23" t="s">
         <v>61</v>
       </c>
@@ -9286,7 +9316,7 @@
       <c r="V62" s="194"/>
     </row>
     <row r="63" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q63" s="235"/>
+      <c r="Q63" s="237"/>
       <c r="R63" s="6" t="s">
         <v>73</v>
       </c>
@@ -9295,7 +9325,7 @@
       <c r="U63" s="30"/>
     </row>
     <row r="64" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q64" s="235"/>
+      <c r="Q64" s="237"/>
       <c r="R64" s="23" t="s">
         <v>74</v>
       </c>
@@ -9310,7 +9340,7 @@
       </c>
     </row>
     <row r="65" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q65" s="236"/>
+      <c r="Q65" s="238"/>
       <c r="R65" s="40" t="s">
         <v>77</v>
       </c>
@@ -9325,7 +9355,7 @@
       </c>
     </row>
     <row r="66" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q66" s="234" t="s">
+      <c r="Q66" s="236" t="s">
         <v>346</v>
       </c>
       <c r="R66" s="18" t="s">
@@ -9338,7 +9368,7 @@
       <c r="U66" s="21"/>
     </row>
     <row r="67" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q67" s="235"/>
+      <c r="Q67" s="237"/>
       <c r="R67" s="6" t="s">
         <v>83</v>
       </c>
@@ -9347,7 +9377,7 @@
       <c r="U67" s="30"/>
     </row>
     <row r="68" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q68" s="235"/>
+      <c r="Q68" s="237"/>
       <c r="R68" s="23" t="s">
         <v>81</v>
       </c>
@@ -9360,7 +9390,7 @@
       <c r="U68" s="45"/>
     </row>
     <row r="69" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q69" s="235"/>
+      <c r="Q69" s="237"/>
       <c r="R69" s="2" t="s">
         <v>86</v>
       </c>
@@ -9373,7 +9403,7 @@
       </c>
     </row>
     <row r="70" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q70" s="235"/>
+      <c r="Q70" s="237"/>
       <c r="R70" s="6" t="s">
         <v>84</v>
       </c>
@@ -9382,7 +9412,7 @@
       <c r="U70" s="49"/>
     </row>
     <row r="71" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q71" s="235"/>
+      <c r="Q71" s="237"/>
       <c r="R71" s="23" t="s">
         <v>85</v>
       </c>
@@ -9395,7 +9425,7 @@
       <c r="U71" s="45"/>
     </row>
     <row r="72" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q72" s="235"/>
+      <c r="Q72" s="237"/>
       <c r="R72" s="23" t="s">
         <v>89</v>
       </c>
@@ -9410,7 +9440,7 @@
       </c>
     </row>
     <row r="73" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q73" s="236"/>
+      <c r="Q73" s="238"/>
       <c r="R73" s="40"/>
       <c r="S73" s="41" t="s">
         <v>88</v>
@@ -9468,20 +9498,20 @@
   <sheetData>
     <row r="1" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="237" t="s">
+      <c r="J2" s="239" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="238"/>
-      <c r="L2" s="238"/>
-      <c r="M2" s="238"/>
-      <c r="N2" s="239"/>
-      <c r="Q2" s="237" t="s">
+      <c r="K2" s="240"/>
+      <c r="L2" s="240"/>
+      <c r="M2" s="240"/>
+      <c r="N2" s="241"/>
+      <c r="Q2" s="239" t="s">
         <v>336</v>
       </c>
-      <c r="R2" s="238"/>
-      <c r="S2" s="238"/>
-      <c r="T2" s="238"/>
-      <c r="U2" s="239"/>
+      <c r="R2" s="240"/>
+      <c r="S2" s="240"/>
+      <c r="T2" s="240"/>
+      <c r="U2" s="241"/>
     </row>
     <row r="3" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J3" s="11"/>
@@ -9493,7 +9523,7 @@
       <c r="N3" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="Q3" s="243" t="s">
+      <c r="Q3" s="245" t="s">
         <v>3</v>
       </c>
       <c r="R3" s="18" t="s">
@@ -9520,7 +9550,7 @@
         <f>M4/25.4</f>
         <v>52.5</v>
       </c>
-      <c r="Q4" s="244"/>
+      <c r="Q4" s="246"/>
       <c r="R4" s="1"/>
       <c r="S4" s="166"/>
       <c r="T4" s="2"/>
@@ -9540,7 +9570,7 @@
         <f>M5/25.4</f>
         <v>48.031496062992126</v>
       </c>
-      <c r="Q5" s="244"/>
+      <c r="Q5" s="246"/>
       <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
@@ -9562,7 +9592,7 @@
         <f t="shared" ref="N6:N7" si="0">M6/25.4</f>
         <v>6.0000000000000009</v>
       </c>
-      <c r="Q6" s="244"/>
+      <c r="Q6" s="246"/>
       <c r="R6" s="23" t="s">
         <v>6</v>
       </c>
@@ -9584,7 +9614,7 @@
         <f t="shared" si="0"/>
         <v>12.000000000000002</v>
       </c>
-      <c r="Q7" s="244"/>
+      <c r="Q7" s="246"/>
       <c r="R7" s="23" t="s">
         <v>7</v>
       </c>
@@ -9612,7 +9642,7 @@
         <f>M8/25.4</f>
         <v>9</v>
       </c>
-      <c r="Q8" s="244"/>
+      <c r="Q8" s="246"/>
       <c r="R8" s="23" t="s">
         <v>10</v>
       </c>
@@ -9637,7 +9667,7 @@
       <c r="N9" s="200" t="s">
         <v>352</v>
       </c>
-      <c r="Q9" s="244"/>
+      <c r="Q9" s="246"/>
       <c r="R9" s="3" t="s">
         <v>11</v>
       </c>
@@ -9650,7 +9680,7 @@
       <c r="U9" s="29"/>
     </row>
     <row r="10" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q10" s="244"/>
+      <c r="Q10" s="246"/>
       <c r="R10" s="6" t="s">
         <v>13</v>
       </c>
@@ -9659,14 +9689,14 @@
       <c r="U10" s="30"/>
     </row>
     <row r="11" spans="10:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="240" t="s">
+      <c r="J11" s="242" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="241"/>
-      <c r="L11" s="241"/>
-      <c r="M11" s="241"/>
-      <c r="N11" s="242"/>
-      <c r="Q11" s="244"/>
+      <c r="K11" s="243"/>
+      <c r="L11" s="243"/>
+      <c r="M11" s="243"/>
+      <c r="N11" s="244"/>
+      <c r="Q11" s="246"/>
       <c r="R11" s="23" t="s">
         <v>6</v>
       </c>
@@ -9690,7 +9720,7 @@
       <c r="N12" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="Q12" s="244"/>
+      <c r="Q12" s="246"/>
       <c r="R12" s="23" t="s">
         <v>7</v>
       </c>
@@ -9723,7 +9753,7 @@
         <f>M13/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="244"/>
+      <c r="Q13" s="246"/>
       <c r="R13" s="23" t="s">
         <v>10</v>
       </c>
@@ -9752,7 +9782,7 @@
         <f t="shared" ref="N14:N32" si="2">M14/25.4</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="244"/>
+      <c r="Q14" s="246"/>
       <c r="R14" s="3" t="s">
         <v>11</v>
       </c>
@@ -9784,7 +9814,7 @@
         <v>6.2143700787401581</v>
       </c>
       <c r="O15" s="178"/>
-      <c r="Q15" s="244"/>
+      <c r="Q15" s="246"/>
       <c r="R15" s="6" t="s">
         <v>16</v>
       </c>
@@ -9811,7 +9841,7 @@
         <f t="shared" si="2"/>
         <v>6.2143700787401581</v>
       </c>
-      <c r="Q16" s="244"/>
+      <c r="Q16" s="246"/>
       <c r="R16" s="23" t="s">
         <v>6</v>
       </c>
@@ -9839,7 +9869,7 @@
         <v>12.428543307086615</v>
       </c>
       <c r="O17" s="178"/>
-      <c r="Q17" s="244"/>
+      <c r="Q17" s="246"/>
       <c r="R17" s="23" t="s">
         <v>7</v>
       </c>
@@ -9872,7 +9902,7 @@
         <f t="shared" si="2"/>
         <v>12.428543307086615</v>
       </c>
-      <c r="Q18" s="244"/>
+      <c r="Q18" s="246"/>
       <c r="R18" s="23" t="s">
         <v>10</v>
       </c>
@@ -9902,7 +9932,7 @@
         <v>18.642913385826773</v>
       </c>
       <c r="O19" s="178"/>
-      <c r="Q19" s="244"/>
+      <c r="Q19" s="246"/>
       <c r="R19" s="3" t="s">
         <v>11</v>
       </c>
@@ -9934,7 +9964,7 @@
         <f t="shared" si="2"/>
         <v>18.642913385826773</v>
       </c>
-      <c r="Q20" s="244"/>
+      <c r="Q20" s="246"/>
       <c r="R20" s="32" t="s">
         <v>19</v>
       </c>
@@ -9968,7 +9998,7 @@
         <v>24.85708661417323</v>
       </c>
       <c r="O21" s="178"/>
-      <c r="Q21" s="244"/>
+      <c r="Q21" s="246"/>
       <c r="R21" s="32" t="s">
         <v>21</v>
       </c>
@@ -9999,7 +10029,7 @@
         <f t="shared" si="2"/>
         <v>24.85708661417323</v>
       </c>
-      <c r="Q22" s="244"/>
+      <c r="Q22" s="246"/>
       <c r="R22" s="32" t="s">
         <v>24</v>
       </c>
@@ -10031,7 +10061,7 @@
         <v>31.07145669291339</v>
       </c>
       <c r="O23" s="178"/>
-      <c r="Q23" s="245"/>
+      <c r="Q23" s="247"/>
       <c r="R23" s="2"/>
       <c r="S23" s="8" t="s">
         <v>26</v>
@@ -10060,7 +10090,7 @@
         <f t="shared" si="2"/>
         <v>31.07145669291339</v>
       </c>
-      <c r="Q24" s="246" t="s">
+      <c r="Q24" s="248" t="s">
         <v>27</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -10092,7 +10122,7 @@
         <v>37.28562992125984</v>
       </c>
       <c r="O25" s="178"/>
-      <c r="Q25" s="244"/>
+      <c r="Q25" s="246"/>
       <c r="R25" s="6" t="s">
         <v>29</v>
       </c>
@@ -10119,7 +10149,7 @@
         <f t="shared" si="2"/>
         <v>37.28562992125984</v>
       </c>
-      <c r="Q26" s="244"/>
+      <c r="Q26" s="246"/>
       <c r="R26" s="23" t="s">
         <v>30</v>
       </c>
@@ -10153,7 +10183,7 @@
         <v>43.500000000000007</v>
       </c>
       <c r="O27" s="178"/>
-      <c r="Q27" s="244"/>
+      <c r="Q27" s="246"/>
       <c r="R27" s="23" t="s">
         <v>32</v>
       </c>
@@ -10184,7 +10214,7 @@
         <f t="shared" si="2"/>
         <v>43.500000000000007</v>
       </c>
-      <c r="Q28" s="244"/>
+      <c r="Q28" s="246"/>
       <c r="R28" s="23" t="s">
         <v>19</v>
       </c>
@@ -10219,7 +10249,7 @@
         <v>48.000000000000007</v>
       </c>
       <c r="O29" s="178"/>
-      <c r="Q29" s="244"/>
+      <c r="Q29" s="246"/>
       <c r="R29" s="23" t="s">
         <v>34</v>
       </c>
@@ -10251,7 +10281,7 @@
         <f t="shared" si="2"/>
         <v>48.000000000000007</v>
       </c>
-      <c r="Q30" s="244"/>
+      <c r="Q30" s="246"/>
       <c r="R30" s="23" t="s">
         <v>36</v>
       </c>
@@ -10284,7 +10314,7 @@
         <v>52.5</v>
       </c>
       <c r="O31" s="178"/>
-      <c r="Q31" s="244"/>
+      <c r="Q31" s="246"/>
       <c r="R31" s="6" t="s">
         <v>37</v>
       </c>
@@ -10311,7 +10341,7 @@
         <f t="shared" si="2"/>
         <v>52.5</v>
       </c>
-      <c r="Q32" s="244"/>
+      <c r="Q32" s="246"/>
       <c r="R32" s="23" t="s">
         <v>38</v>
       </c>
@@ -10326,7 +10356,7 @@
       </c>
     </row>
     <row r="33" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q33" s="244"/>
+      <c r="Q33" s="246"/>
       <c r="R33" s="23" t="s">
         <v>40</v>
       </c>
@@ -10339,7 +10369,7 @@
       <c r="U33" s="25"/>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q34" s="244"/>
+      <c r="Q34" s="246"/>
       <c r="R34" s="23" t="s">
         <v>42</v>
       </c>
@@ -10355,7 +10385,7 @@
       </c>
     </row>
     <row r="35" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q35" s="244"/>
+      <c r="Q35" s="246"/>
       <c r="R35" s="23" t="s">
         <v>34</v>
       </c>
@@ -10368,7 +10398,7 @@
       <c r="U35" s="25"/>
     </row>
     <row r="36" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q36" s="244"/>
+      <c r="Q36" s="246"/>
       <c r="R36" s="23" t="s">
         <v>36</v>
       </c>
@@ -10382,7 +10412,7 @@
       <c r="U36" s="190"/>
     </row>
     <row r="37" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q37" s="244"/>
+      <c r="Q37" s="246"/>
       <c r="R37" s="6" t="s">
         <v>44</v>
       </c>
@@ -10391,7 +10421,7 @@
       <c r="U37" s="30"/>
     </row>
     <row r="38" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q38" s="244"/>
+      <c r="Q38" s="246"/>
       <c r="R38" s="23" t="s">
         <v>45</v>
       </c>
@@ -10407,7 +10437,7 @@
       </c>
     </row>
     <row r="39" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q39" s="244"/>
+      <c r="Q39" s="246"/>
       <c r="R39" s="23" t="s">
         <v>46</v>
       </c>
@@ -10420,7 +10450,7 @@
       <c r="U39" s="25"/>
     </row>
     <row r="40" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="244"/>
+      <c r="Q40" s="246"/>
       <c r="R40" s="23" t="s">
         <v>34</v>
       </c>
@@ -10435,7 +10465,7 @@
       </c>
     </row>
     <row r="41" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="245"/>
+      <c r="Q41" s="247"/>
       <c r="R41" s="23" t="s">
         <v>36</v>
       </c>
@@ -10448,7 +10478,7 @@
       <c r="U41" s="22"/>
     </row>
     <row r="42" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q42" s="247" t="s">
+      <c r="Q42" s="249" t="s">
         <v>50</v>
       </c>
       <c r="R42" s="6" t="s">
@@ -10461,7 +10491,7 @@
       <c r="U42" s="30"/>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q43" s="235"/>
+      <c r="Q43" s="237"/>
       <c r="R43" s="6" t="s">
         <v>52</v>
       </c>
@@ -10470,7 +10500,7 @@
       <c r="U43" s="30"/>
     </row>
     <row r="44" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q44" s="235"/>
+      <c r="Q44" s="237"/>
       <c r="R44" s="23" t="s">
         <v>53</v>
       </c>
@@ -10481,7 +10511,7 @@
       <c r="U44" s="25"/>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q45" s="235"/>
+      <c r="Q45" s="237"/>
       <c r="R45" s="23" t="s">
         <v>54</v>
       </c>
@@ -10496,7 +10526,7 @@
       </c>
     </row>
     <row r="46" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q46" s="235"/>
+      <c r="Q46" s="237"/>
       <c r="R46" s="23" t="s">
         <v>57</v>
       </c>
@@ -10511,7 +10541,7 @@
       </c>
     </row>
     <row r="47" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q47" s="235"/>
+      <c r="Q47" s="237"/>
       <c r="R47" s="23" t="s">
         <v>59</v>
       </c>
@@ -10527,7 +10557,7 @@
       </c>
     </row>
     <row r="48" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q48" s="235"/>
+      <c r="Q48" s="237"/>
       <c r="R48" s="23"/>
       <c r="S48" s="26" t="s">
         <v>306</v>
@@ -10539,7 +10569,7 @@
       <c r="U48" s="25"/>
     </row>
     <row r="49" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q49" s="235"/>
+      <c r="Q49" s="237"/>
       <c r="R49" s="23" t="s">
         <v>61</v>
       </c>
@@ -10553,7 +10583,7 @@
       <c r="U49" s="25"/>
     </row>
     <row r="50" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q50" s="235"/>
+      <c r="Q50" s="237"/>
       <c r="R50" s="6" t="s">
         <v>62</v>
       </c>
@@ -10565,7 +10595,7 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="Q51" s="235"/>
+      <c r="Q51" s="237"/>
       <c r="R51" s="23" t="s">
         <v>63</v>
       </c>
@@ -10580,7 +10610,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="N52" s="144"/>
-      <c r="Q52" s="235"/>
+      <c r="Q52" s="237"/>
       <c r="R52" s="23" t="s">
         <v>54</v>
       </c>
@@ -10598,7 +10628,7 @@
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
-      <c r="Q53" s="235"/>
+      <c r="Q53" s="237"/>
       <c r="R53" s="23" t="s">
         <v>64</v>
       </c>
@@ -10614,7 +10644,7 @@
       </c>
     </row>
     <row r="54" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q54" s="235"/>
+      <c r="Q54" s="237"/>
       <c r="R54" s="23" t="s">
         <v>66</v>
       </c>
@@ -10630,7 +10660,7 @@
       </c>
     </row>
     <row r="55" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q55" s="235"/>
+      <c r="Q55" s="237"/>
       <c r="R55" s="23" t="s">
         <v>61</v>
       </c>
@@ -10644,7 +10674,7 @@
       <c r="U55" s="25"/>
     </row>
     <row r="56" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q56" s="235"/>
+      <c r="Q56" s="237"/>
       <c r="R56" s="6" t="s">
         <v>69</v>
       </c>
@@ -10653,7 +10683,7 @@
       <c r="U56" s="30"/>
     </row>
     <row r="57" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q57" s="235"/>
+      <c r="Q57" s="237"/>
       <c r="R57" s="23" t="s">
         <v>70</v>
       </c>
@@ -10664,7 +10694,7 @@
       <c r="U57" s="25"/>
     </row>
     <row r="58" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q58" s="235"/>
+      <c r="Q58" s="237"/>
       <c r="R58" s="23" t="s">
         <v>54</v>
       </c>
@@ -10680,7 +10710,7 @@
       <c r="V58" s="27"/>
     </row>
     <row r="59" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q59" s="235"/>
+      <c r="Q59" s="237"/>
       <c r="R59" s="23" t="s">
         <v>57</v>
       </c>
@@ -10695,7 +10725,7 @@
       </c>
     </row>
     <row r="60" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q60" s="235"/>
+      <c r="Q60" s="237"/>
       <c r="R60" s="23" t="s">
         <v>71</v>
       </c>
@@ -10708,7 +10738,7 @@
       <c r="U60" s="25"/>
     </row>
     <row r="61" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q61" s="235"/>
+      <c r="Q61" s="237"/>
       <c r="R61" s="23" t="s">
         <v>59</v>
       </c>
@@ -10725,7 +10755,7 @@
       <c r="V61" s="37"/>
     </row>
     <row r="62" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q62" s="235"/>
+      <c r="Q62" s="237"/>
       <c r="R62" s="23" t="s">
         <v>61</v>
       </c>
@@ -10740,7 +10770,7 @@
       <c r="V62" s="194"/>
     </row>
     <row r="63" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q63" s="235"/>
+      <c r="Q63" s="237"/>
       <c r="R63" s="6" t="s">
         <v>73</v>
       </c>
@@ -10749,7 +10779,7 @@
       <c r="U63" s="30"/>
     </row>
     <row r="64" spans="8:22" x14ac:dyDescent="0.25">
-      <c r="Q64" s="235"/>
+      <c r="Q64" s="237"/>
       <c r="R64" s="23" t="s">
         <v>74</v>
       </c>
@@ -10764,7 +10794,7 @@
       </c>
     </row>
     <row r="65" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q65" s="236"/>
+      <c r="Q65" s="238"/>
       <c r="R65" s="40" t="s">
         <v>77</v>
       </c>
@@ -10779,7 +10809,7 @@
       </c>
     </row>
     <row r="66" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q66" s="234" t="s">
+      <c r="Q66" s="236" t="s">
         <v>346</v>
       </c>
       <c r="R66" s="18" t="s">
@@ -10792,7 +10822,7 @@
       <c r="U66" s="21"/>
     </row>
     <row r="67" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q67" s="235"/>
+      <c r="Q67" s="237"/>
       <c r="R67" s="6" t="s">
         <v>83</v>
       </c>
@@ -10801,7 +10831,7 @@
       <c r="U67" s="30"/>
     </row>
     <row r="68" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q68" s="235"/>
+      <c r="Q68" s="237"/>
       <c r="R68" s="23" t="s">
         <v>81</v>
       </c>
@@ -10814,7 +10844,7 @@
       <c r="U68" s="45"/>
     </row>
     <row r="69" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q69" s="235"/>
+      <c r="Q69" s="237"/>
       <c r="R69" s="2" t="s">
         <v>86</v>
       </c>
@@ -10827,7 +10857,7 @@
       </c>
     </row>
     <row r="70" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q70" s="235"/>
+      <c r="Q70" s="237"/>
       <c r="R70" s="6" t="s">
         <v>84</v>
       </c>
@@ -10836,7 +10866,7 @@
       <c r="U70" s="49"/>
     </row>
     <row r="71" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q71" s="235"/>
+      <c r="Q71" s="237"/>
       <c r="R71" s="23" t="s">
         <v>85</v>
       </c>
@@ -10849,7 +10879,7 @@
       <c r="U71" s="45"/>
     </row>
     <row r="72" spans="17:21" x14ac:dyDescent="0.25">
-      <c r="Q72" s="235"/>
+      <c r="Q72" s="237"/>
       <c r="R72" s="23" t="s">
         <v>89</v>
       </c>
@@ -10864,7 +10894,7 @@
       </c>
     </row>
     <row r="73" spans="17:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q73" s="236"/>
+      <c r="Q73" s="238"/>
       <c r="R73" s="40"/>
       <c r="S73" s="41" t="s">
         <v>88</v>
@@ -10896,14 +10926,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE64495-0A64-4917-8E7B-BBB41A05E68F}">
-  <dimension ref="H3:Z66"/>
+  <dimension ref="H3:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" topLeftCell="G50" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="9" max="9" width="14.77734375" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
@@ -10917,20 +10948,25 @@
     <col min="23" max="23" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.77734375" customWidth="1"/>
+    <col min="29" max="29" width="8.44140625" customWidth="1"/>
+    <col min="30" max="30" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="9:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="9:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I4" s="240" t="s">
+    <row r="3" spans="9:34" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="9:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="242" t="s">
         <v>80</v>
       </c>
-      <c r="J4" s="241"/>
-      <c r="K4" s="241"/>
-      <c r="L4" s="241"/>
-      <c r="M4" s="242"/>
-    </row>
-    <row r="5" spans="9:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4" s="243"/>
+      <c r="K4" s="243"/>
+      <c r="L4" s="243"/>
+      <c r="M4" s="244"/>
+    </row>
+    <row r="5" spans="9:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I5" s="11" t="s">
         <v>90</v>
       </c>
@@ -10946,15 +10982,29 @@
       <c r="M5" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="P5" s="240" t="s">
+      <c r="P5" s="242" t="s">
         <v>80</v>
       </c>
-      <c r="Q5" s="241"/>
-      <c r="R5" s="241"/>
-      <c r="S5" s="241"/>
-      <c r="T5" s="242"/>
-    </row>
-    <row r="6" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Q5" s="243"/>
+      <c r="R5" s="243"/>
+      <c r="S5" s="243"/>
+      <c r="T5" s="244"/>
+      <c r="V5" s="289" t="s">
+        <v>380</v>
+      </c>
+      <c r="W5" s="290"/>
+      <c r="X5" s="290"/>
+      <c r="Y5" s="290"/>
+      <c r="Z5" s="291"/>
+      <c r="AC5" s="278" t="s">
+        <v>381</v>
+      </c>
+      <c r="AD5" s="279"/>
+      <c r="AE5" s="279"/>
+      <c r="AF5" s="279"/>
+      <c r="AG5" s="280"/>
+    </row>
+    <row r="6" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I6" s="14">
         <v>1</v>
       </c>
@@ -10987,23 +11037,38 @@
       <c r="T6" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="V6" s="97" t="s">
         <v>90</v>
       </c>
-      <c r="W6" s="12" t="s">
+      <c r="W6" s="98" t="s">
         <v>327</v>
       </c>
-      <c r="X6" s="12" t="s">
+      <c r="X6" s="98" t="s">
         <v>311</v>
       </c>
-      <c r="Y6" s="12" t="s">
+      <c r="Y6" s="98" t="s">
         <v>328</v>
       </c>
-      <c r="Z6" s="13" t="s">
+      <c r="Z6" s="99" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="7" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="AC6" s="97" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD6" s="98" t="s">
+        <v>327</v>
+      </c>
+      <c r="AE6" s="98" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF6" s="98" t="s">
+        <v>328</v>
+      </c>
+      <c r="AG6" s="99" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I7" s="14">
         <v>2</v>
       </c>
@@ -11038,14 +11103,26 @@
         <f>S7/25.4</f>
         <v>0</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="227">
         <v>1</v>
       </c>
-      <c r="Y7">
+      <c r="W7" s="285"/>
+      <c r="X7" s="285"/>
+      <c r="Y7" s="285">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z7" s="57"/>
+      <c r="AC7" s="227">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="285"/>
+      <c r="AE7" s="285"/>
+      <c r="AF7" s="285">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="57"/>
+    </row>
+    <row r="8" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I8" s="14">
         <v>3</v>
       </c>
@@ -11084,14 +11161,26 @@
         <f t="shared" ref="T8:T26" si="3">S8/25.4</f>
         <v>0</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="227">
         <v>2</v>
       </c>
-      <c r="Y8">
+      <c r="W8" s="285"/>
+      <c r="X8" s="285"/>
+      <c r="Y8" s="285">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z8" s="57"/>
+      <c r="AC8" s="227">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="285"/>
+      <c r="AE8" s="285"/>
+      <c r="AF8" s="285">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="57"/>
+    </row>
+    <row r="9" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I9" s="14">
         <v>4</v>
       </c>
@@ -11127,14 +11216,34 @@
         <f t="shared" si="3"/>
         <v>12.428740157480316</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="227">
         <v>3</v>
       </c>
-      <c r="Y9">
+      <c r="W9" s="285"/>
+      <c r="X9" s="285"/>
+      <c r="Y9" s="285">
         <v>610</v>
       </c>
-    </row>
-    <row r="10" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z9" s="57"/>
+      <c r="AA9">
+        <f>Y9-Y9/2</f>
+        <v>305</v>
+      </c>
+      <c r="AC9" s="227">
+        <v>3</v>
+      </c>
+      <c r="AD9" s="285"/>
+      <c r="AE9" s="285"/>
+      <c r="AF9" s="285">
+        <v>305</v>
+      </c>
+      <c r="AG9" s="57"/>
+      <c r="AH9">
+        <f>AF9-AF9/2</f>
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="10" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I10" s="14">
         <v>5</v>
       </c>
@@ -11173,14 +11282,26 @@
         <f t="shared" si="3"/>
         <v>12.428740157480316</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="227">
         <v>4</v>
       </c>
-      <c r="Y10">
+      <c r="W10" s="285"/>
+      <c r="X10" s="285"/>
+      <c r="Y10" s="285">
         <v>610</v>
       </c>
-    </row>
-    <row r="11" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z10" s="57"/>
+      <c r="AC10" s="227">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="285"/>
+      <c r="AE10" s="285"/>
+      <c r="AF10" s="285">
+        <v>305</v>
+      </c>
+      <c r="AG10" s="57"/>
+    </row>
+    <row r="11" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I11" s="14">
         <v>6</v>
       </c>
@@ -11216,15 +11337,36 @@
         <f t="shared" si="3"/>
         <v>24.85708661417323</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="227">
         <v>5</v>
       </c>
-      <c r="Y11">
+      <c r="W11" s="285"/>
+      <c r="X11" s="285"/>
+      <c r="Y11" s="285">
         <f>Y9+S31</f>
         <v>929.96</v>
       </c>
-    </row>
-    <row r="12" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z11" s="57"/>
+      <c r="AA11">
+        <f>Y11-319.96/2</f>
+        <v>769.98</v>
+      </c>
+      <c r="AC11" s="227">
+        <v>5</v>
+      </c>
+      <c r="AD11" s="285"/>
+      <c r="AE11" s="285"/>
+      <c r="AF11" s="285">
+        <f>AF9*2</f>
+        <v>610</v>
+      </c>
+      <c r="AG11" s="57"/>
+      <c r="AH11">
+        <f>AF11-AF9/2</f>
+        <v>457.5</v>
+      </c>
+    </row>
+    <row r="12" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I12" s="14">
         <v>7</v>
       </c>
@@ -11263,15 +11405,28 @@
         <f t="shared" si="3"/>
         <v>24.85708661417323</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="227">
         <v>6</v>
       </c>
-      <c r="Y12">
+      <c r="W12" s="285"/>
+      <c r="X12" s="285"/>
+      <c r="Y12" s="285">
         <f>Y11</f>
         <v>929.96</v>
       </c>
-    </row>
-    <row r="13" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z12" s="57"/>
+      <c r="AC12" s="227">
+        <v>6</v>
+      </c>
+      <c r="AD12" s="285"/>
+      <c r="AE12" s="285"/>
+      <c r="AF12" s="285">
+        <f>AF11</f>
+        <v>610</v>
+      </c>
+      <c r="AG12" s="57"/>
+    </row>
+    <row r="13" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I13" s="14">
         <v>8</v>
       </c>
@@ -11307,15 +11462,36 @@
         <f t="shared" si="3"/>
         <v>37.285826771653547</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="227">
         <v>7</v>
       </c>
-      <c r="Y13">
+      <c r="W13" s="285"/>
+      <c r="X13" s="285"/>
+      <c r="Y13" s="285">
         <f>Y11+S31</f>
         <v>1249.92</v>
       </c>
-    </row>
-    <row r="14" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z13" s="57"/>
+      <c r="AA13">
+        <f>Y13-319.96/2</f>
+        <v>1089.94</v>
+      </c>
+      <c r="AC13" s="227">
+        <v>7</v>
+      </c>
+      <c r="AD13" s="285"/>
+      <c r="AE13" s="285"/>
+      <c r="AF13" s="285">
+        <f>AF11+S31</f>
+        <v>929.96</v>
+      </c>
+      <c r="AG13" s="57"/>
+      <c r="AH13">
+        <f>AF13-319.96/2</f>
+        <v>769.98</v>
+      </c>
+    </row>
+    <row r="14" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I14" s="14">
         <v>9</v>
       </c>
@@ -11354,15 +11530,28 @@
         <f t="shared" si="3"/>
         <v>37.285826771653547</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="227">
         <v>8</v>
       </c>
-      <c r="Y14">
+      <c r="W14" s="285"/>
+      <c r="X14" s="285"/>
+      <c r="Y14" s="285">
         <f>Y13</f>
         <v>1249.92</v>
       </c>
-    </row>
-    <row r="15" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z14" s="57"/>
+      <c r="AC14" s="227">
+        <v>8</v>
+      </c>
+      <c r="AD14" s="285"/>
+      <c r="AE14" s="285"/>
+      <c r="AF14" s="285">
+        <f>AF13</f>
+        <v>929.96</v>
+      </c>
+      <c r="AG14" s="57"/>
+    </row>
+    <row r="15" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I15" s="14">
         <v>10</v>
       </c>
@@ -11398,15 +11587,36 @@
         <f t="shared" si="3"/>
         <v>49.714173228346461</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="227">
         <v>9</v>
       </c>
-      <c r="Y15">
+      <c r="W15" s="285"/>
+      <c r="X15" s="285"/>
+      <c r="Y15" s="285">
         <f>Y13+S31</f>
         <v>1569.88</v>
       </c>
-    </row>
-    <row r="16" spans="9:26" x14ac:dyDescent="0.3">
+      <c r="Z15" s="57"/>
+      <c r="AA15">
+        <f>Y15-319.96/2</f>
+        <v>1409.9</v>
+      </c>
+      <c r="AC15" s="227">
+        <v>9</v>
+      </c>
+      <c r="AD15" s="285"/>
+      <c r="AE15" s="285"/>
+      <c r="AF15" s="285">
+        <f>AF13+S31</f>
+        <v>1249.92</v>
+      </c>
+      <c r="AG15" s="57"/>
+      <c r="AH15">
+        <f>AF15-319.96/2</f>
+        <v>1089.94</v>
+      </c>
+    </row>
+    <row r="16" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I16" s="14">
         <v>11</v>
       </c>
@@ -11445,15 +11655,28 @@
         <f t="shared" si="3"/>
         <v>49.714173228346461</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="227">
         <v>10</v>
       </c>
-      <c r="Y16">
+      <c r="W16" s="285"/>
+      <c r="X16" s="285"/>
+      <c r="Y16" s="285">
         <f>Y15</f>
         <v>1569.88</v>
       </c>
-    </row>
-    <row r="17" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z16" s="57"/>
+      <c r="AC16" s="227">
+        <v>10</v>
+      </c>
+      <c r="AD16" s="285"/>
+      <c r="AE16" s="285"/>
+      <c r="AF16" s="285">
+        <f>AF15</f>
+        <v>1249.92</v>
+      </c>
+      <c r="AG16" s="57"/>
+    </row>
+    <row r="17" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I17" s="14">
         <v>12</v>
       </c>
@@ -11489,15 +11712,36 @@
         <f t="shared" si="3"/>
         <v>62.14291338582678</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="227">
         <v>11</v>
       </c>
-      <c r="Y17">
+      <c r="W17" s="285"/>
+      <c r="X17" s="285"/>
+      <c r="Y17" s="285">
         <f>Y15+S31</f>
         <v>1889.8400000000001</v>
       </c>
-    </row>
-    <row r="18" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z17" s="57"/>
+      <c r="AA17">
+        <f>Y17-319.96/2</f>
+        <v>1729.8600000000001</v>
+      </c>
+      <c r="AC17" s="227">
+        <v>11</v>
+      </c>
+      <c r="AD17" s="285"/>
+      <c r="AE17" s="285"/>
+      <c r="AF17" s="285">
+        <f>AF15+S31</f>
+        <v>1569.88</v>
+      </c>
+      <c r="AG17" s="57"/>
+      <c r="AH17">
+        <f>AF17-319.96/2</f>
+        <v>1409.9</v>
+      </c>
+    </row>
+    <row r="18" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I18" s="232">
         <v>13</v>
       </c>
@@ -11536,15 +11780,28 @@
         <f t="shared" si="3"/>
         <v>62.14291338582678</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="227">
         <v>12</v>
       </c>
-      <c r="Y18">
+      <c r="W18" s="285"/>
+      <c r="X18" s="285"/>
+      <c r="Y18" s="285">
         <f>Y17</f>
         <v>1889.8400000000001</v>
       </c>
-    </row>
-    <row r="19" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z18" s="57"/>
+      <c r="AC18" s="227">
+        <v>12</v>
+      </c>
+      <c r="AD18" s="285"/>
+      <c r="AE18" s="285"/>
+      <c r="AF18" s="285">
+        <f>AF17</f>
+        <v>1569.88</v>
+      </c>
+      <c r="AG18" s="57"/>
+    </row>
+    <row r="19" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I19" s="232">
         <v>14</v>
       </c>
@@ -11580,15 +11837,36 @@
         <f t="shared" si="3"/>
         <v>74.57125984251968</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="227">
         <v>13</v>
       </c>
-      <c r="Y19">
+      <c r="W19" s="285"/>
+      <c r="X19" s="285"/>
+      <c r="Y19" s="285">
         <f>Y17+S31</f>
         <v>2209.8000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z19" s="57"/>
+      <c r="AA19">
+        <f>Y19-319.96/2</f>
+        <v>2049.8200000000002</v>
+      </c>
+      <c r="AC19" s="227">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="285"/>
+      <c r="AE19" s="285"/>
+      <c r="AF19" s="285">
+        <f>AF17+S31</f>
+        <v>1889.8400000000001</v>
+      </c>
+      <c r="AG19" s="57"/>
+      <c r="AH19">
+        <f>AF19-319.96/2</f>
+        <v>1729.8600000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I20" s="14">
         <v>15</v>
       </c>
@@ -11621,15 +11899,28 @@
         <f t="shared" si="3"/>
         <v>74.57125984251968</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="227">
         <v>14</v>
       </c>
-      <c r="Y20">
+      <c r="W20" s="285"/>
+      <c r="X20" s="285"/>
+      <c r="Y20" s="285">
         <f>Y19</f>
         <v>2209.8000000000002</v>
       </c>
-    </row>
-    <row r="21" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z20" s="57"/>
+      <c r="AC20" s="227">
+        <v>14</v>
+      </c>
+      <c r="AD20" s="285"/>
+      <c r="AE20" s="285"/>
+      <c r="AF20" s="285">
+        <f>AF19</f>
+        <v>1889.8400000000001</v>
+      </c>
+      <c r="AG20" s="57"/>
+    </row>
+    <row r="21" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I21" s="14">
         <v>16</v>
       </c>
@@ -11662,17 +11953,36 @@
         <f t="shared" si="3"/>
         <v>87.000000000000014</v>
       </c>
-      <c r="V21" s="283">
+      <c r="V21" s="286">
         <v>15</v>
       </c>
-      <c r="W21" s="283"/>
-      <c r="X21" s="283"/>
-      <c r="Y21" s="283">
+      <c r="W21" s="287"/>
+      <c r="X21" s="287"/>
+      <c r="Y21" s="287">
         <f>Y19+S33</f>
         <v>2438.4</v>
       </c>
-    </row>
-    <row r="22" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z21" s="57"/>
+      <c r="AA21">
+        <f>Y21-228.6/2</f>
+        <v>2324.1</v>
+      </c>
+      <c r="AC21" s="227">
+        <v>15</v>
+      </c>
+      <c r="AD21" s="285"/>
+      <c r="AE21" s="285"/>
+      <c r="AF21" s="285">
+        <f>AF19+S31</f>
+        <v>2209.8000000000002</v>
+      </c>
+      <c r="AG21" s="57"/>
+      <c r="AH21">
+        <f t="shared" ref="AH21" si="4">AF21-319.96/2</f>
+        <v>2049.8200000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I22" s="14">
         <v>17</v>
       </c>
@@ -11705,17 +12015,28 @@
         <f t="shared" si="3"/>
         <v>87.000000000000014</v>
       </c>
-      <c r="V22" s="283">
+      <c r="V22" s="286">
         <v>16</v>
       </c>
-      <c r="W22" s="283"/>
-      <c r="X22" s="283"/>
-      <c r="Y22" s="283">
+      <c r="W22" s="287"/>
+      <c r="X22" s="287"/>
+      <c r="Y22" s="287">
         <f>Y21</f>
         <v>2438.4</v>
       </c>
-    </row>
-    <row r="23" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z22" s="57"/>
+      <c r="AC22" s="227">
+        <v>16</v>
+      </c>
+      <c r="AD22" s="285"/>
+      <c r="AE22" s="285"/>
+      <c r="AF22" s="285">
+        <f>AF21</f>
+        <v>2209.8000000000002</v>
+      </c>
+      <c r="AG22" s="57"/>
+    </row>
+    <row r="23" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I23" s="14">
         <v>18</v>
       </c>
@@ -11748,15 +12069,32 @@
         <f t="shared" si="3"/>
         <v>96.000000000000014</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="227">
         <v>17</v>
       </c>
-      <c r="Y23">
+      <c r="W23" s="285"/>
+      <c r="X23" s="285"/>
+      <c r="Y23" s="285">
         <f>Y21+S33</f>
         <v>2667</v>
       </c>
-    </row>
-    <row r="24" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="Z23" s="57"/>
+      <c r="AC23" s="286">
+        <v>17</v>
+      </c>
+      <c r="AD23" s="287"/>
+      <c r="AE23" s="287"/>
+      <c r="AF23" s="287">
+        <f>AF21+S33</f>
+        <v>2438.4</v>
+      </c>
+      <c r="AG23" s="57"/>
+      <c r="AH23">
+        <f>AF23-228.6/2</f>
+        <v>2324.1</v>
+      </c>
+    </row>
+    <row r="24" spans="9:34" x14ac:dyDescent="0.3">
       <c r="I24" s="14">
         <v>19</v>
       </c>
@@ -11789,15 +12127,28 @@
         <f t="shared" si="3"/>
         <v>96.000000000000014</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="230">
         <v>18</v>
       </c>
-      <c r="Y24">
+      <c r="W24" s="288"/>
+      <c r="X24" s="288"/>
+      <c r="Y24" s="288">
         <f>Y23</f>
         <v>2667</v>
       </c>
-    </row>
-    <row r="25" spans="9:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z24" s="231"/>
+      <c r="AC24" s="286">
+        <v>18</v>
+      </c>
+      <c r="AD24" s="287"/>
+      <c r="AE24" s="287"/>
+      <c r="AF24" s="287">
+        <f>AF23</f>
+        <v>2438.4</v>
+      </c>
+      <c r="AG24" s="57"/>
+    </row>
+    <row r="25" spans="9:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I25" s="16">
         <v>20</v>
       </c>
@@ -11830,8 +12181,18 @@
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="9:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC25" s="227">
+        <v>19</v>
+      </c>
+      <c r="AD25" s="285"/>
+      <c r="AE25" s="285"/>
+      <c r="AF25" s="285">
+        <f>AF23+S33</f>
+        <v>2667</v>
+      </c>
+      <c r="AG25" s="57"/>
+    </row>
+    <row r="26" spans="9:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P26" s="16">
         <v>20</v>
       </c>
@@ -11849,8 +12210,18 @@
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="31" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="AC26" s="230">
+        <v>20</v>
+      </c>
+      <c r="AD26" s="288"/>
+      <c r="AE26" s="288"/>
+      <c r="AF26" s="288">
+        <f>AF25</f>
+        <v>2667</v>
+      </c>
+      <c r="AG26" s="231"/>
+    </row>
+    <row r="31" spans="9:34" x14ac:dyDescent="0.3">
       <c r="S31">
         <f>(2667-610-228.6*2)/5</f>
         <v>319.95999999999998</v>
@@ -11861,110 +12232,134 @@
         <v>228.6</v>
       </c>
     </row>
-    <row r="58" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H58" t="s">
+    <row r="57" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H57" s="292" t="s">
+        <v>382</v>
+      </c>
+      <c r="I57" s="293"/>
+      <c r="J57" s="293"/>
+      <c r="K57" s="294"/>
+    </row>
+    <row r="58" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H58" s="234"/>
+      <c r="I58" s="204" t="s">
         <v>376</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="204" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="59" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H59" t="s">
+      <c r="K58" s="235"/>
+    </row>
+    <row r="59" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H59" s="220" t="s">
         <v>211</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="208">
         <v>47.09</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="208">
         <v>53.78</v>
       </c>
-    </row>
-    <row r="60" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H60" t="s">
+      <c r="K59" s="221" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H60" s="220" t="s">
         <v>372</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="208">
         <v>2.32E-3</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="208">
         <v>3.9699999999999996E-3</v>
       </c>
-      <c r="N60" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="61" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H61" t="s">
+      <c r="K60" s="221"/>
+    </row>
+    <row r="61" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H61" s="220" t="s">
         <v>375</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="208">
         <f>4700*I59^0.5</f>
         <v>32252.412312879791</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="208">
         <f>4700*J59^0.5</f>
         <v>34467.378780522318</v>
       </c>
-      <c r="N61" t="s">
+      <c r="K61" s="221" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="62" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H62" t="s">
+    <row r="62" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H62" s="220" t="s">
         <v>373</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="208">
         <v>610</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="208">
         <v>610</v>
       </c>
-    </row>
-    <row r="63" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H63" t="s">
+      <c r="K62" s="221" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H63" s="220" t="s">
         <v>378</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="208" t="s">
         <v>379</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="208">
         <f>5*(J59/I59-0.85)</f>
         <v>1.4603418984922483</v>
       </c>
-    </row>
-    <row r="64" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H64" t="s">
+      <c r="K63" s="221"/>
+    </row>
+    <row r="64" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H64" s="220" t="s">
         <v>370</v>
       </c>
-      <c r="I64">
+      <c r="I64" s="208">
         <v>87.563000000000002</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="208">
         <f>J63*I64</f>
         <v>127.87191765767673</v>
       </c>
-      <c r="N64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="8:10" x14ac:dyDescent="0.3">
-      <c r="H66" t="s">
+      <c r="K64" s="221" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="65" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H65" s="220"/>
+      <c r="I65" s="208"/>
+      <c r="J65" s="208"/>
+      <c r="K65" s="221"/>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H66" s="234" t="s">
         <v>374</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="204">
         <f>I60-I59/I61+2*(I64/I62)/I59</f>
         <v>6.9566159544933127E-3</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="204">
         <f>J60-0.8*J59/J61+((5/3)*J64/J62)/I59</f>
         <v>1.0141089460168916E-2</v>
       </c>
+      <c r="K66" s="235"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="I4:M4"/>
     <mergeCell ref="P5:T5"/>
+    <mergeCell ref="AC5:AG5"/>
+    <mergeCell ref="H57:K57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11991,10 +12386,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="251" t="s">
+      <c r="C3" s="253" t="s">
         <v>215</v>
       </c>
-      <c r="D3" s="251" t="s">
+      <c r="D3" s="253" t="s">
         <v>91</v>
       </c>
       <c r="E3" s="82">
@@ -12006,8 +12401,8 @@
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
+      <c r="C4" s="253"/>
+      <c r="D4" s="253"/>
       <c r="E4" s="84">
         <f>E3*9.807</f>
         <v>-2145185.2167177605</v>
@@ -12021,7 +12416,7 @@
       </c>
     </row>
     <row r="8" spans="3:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="252">
+      <c r="C8" s="254">
         <v>1</v>
       </c>
       <c r="D8" s="147" t="s">
@@ -12034,7 +12429,7 @@
       <c r="G8" s="150"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="253"/>
+      <c r="C9" s="255"/>
       <c r="D9" s="151" t="s">
         <v>111</v>
       </c>
@@ -12043,7 +12438,7 @@
       <c r="G9" s="153"/>
     </row>
     <row r="10" spans="3:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C10" s="253"/>
+      <c r="C10" s="255"/>
       <c r="D10" s="154" t="s">
         <v>34</v>
       </c>
@@ -12056,7 +12451,7 @@
       <c r="G10" s="157"/>
     </row>
     <row r="11" spans="3:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C11" s="253"/>
+      <c r="C11" s="255"/>
       <c r="D11" s="151" t="s">
         <v>113</v>
       </c>
@@ -12065,7 +12460,7 @@
       <c r="G11" s="157"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="253"/>
+      <c r="C12" s="255"/>
       <c r="D12" s="154" t="s">
         <v>114</v>
       </c>
@@ -12078,7 +12473,7 @@
       <c r="G12" s="153"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="253"/>
+      <c r="C13" s="255"/>
       <c r="D13" s="151" t="s">
         <v>112</v>
       </c>
@@ -12090,7 +12485,7 @@
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="253"/>
+      <c r="C14" s="255"/>
       <c r="D14" s="154" t="s">
         <v>98</v>
       </c>
@@ -12107,7 +12502,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="253"/>
+      <c r="C15" s="255"/>
       <c r="D15" s="154" t="s">
         <v>97</v>
       </c>
@@ -12127,7 +12522,7 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="253"/>
+      <c r="C16" s="255"/>
       <c r="D16" s="154" t="s">
         <v>102</v>
       </c>
@@ -12140,7 +12535,7 @@
       <c r="G16" s="153"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="253"/>
+      <c r="C17" s="255"/>
       <c r="D17" s="154" t="s">
         <v>103</v>
       </c>
@@ -12153,7 +12548,7 @@
       <c r="G17" s="153"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="253"/>
+      <c r="C18" s="255"/>
       <c r="D18" s="154" t="s">
         <v>94</v>
       </c>
@@ -12166,7 +12561,7 @@
       <c r="G18" s="153"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="253"/>
+      <c r="C19" s="255"/>
       <c r="D19" s="161" t="s">
         <v>95</v>
       </c>
@@ -12179,7 +12574,7 @@
       <c r="G19" s="164"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="253"/>
+      <c r="C20" s="255"/>
       <c r="D20" s="147" t="s">
         <v>116</v>
       </c>
@@ -12190,7 +12585,7 @@
       <c r="G20" s="150"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="253"/>
+      <c r="C21" s="255"/>
       <c r="D21" s="154" t="s">
         <v>119</v>
       </c>
@@ -12201,7 +12596,7 @@
       <c r="G21" s="153"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="253"/>
+      <c r="C22" s="255"/>
       <c r="D22" s="161" t="s">
         <v>121</v>
       </c>
@@ -12212,7 +12607,7 @@
       <c r="G22" s="164"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="253"/>
+      <c r="C23" s="255"/>
       <c r="D23" s="147" t="s">
         <v>116</v>
       </c>
@@ -12223,7 +12618,7 @@
       <c r="G23" s="150"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="253"/>
+      <c r="C24" s="255"/>
       <c r="D24" s="154" t="s">
         <v>126</v>
       </c>
@@ -12236,7 +12631,7 @@
       <c r="G24" s="153"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="253"/>
+      <c r="C25" s="255"/>
       <c r="D25" s="154" t="s">
         <v>119</v>
       </c>
@@ -12249,7 +12644,7 @@
       <c r="G25" s="153"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="254"/>
+      <c r="C26" s="256"/>
       <c r="D26" s="161" t="s">
         <v>110</v>
       </c>
@@ -12262,7 +12657,7 @@
       <c r="G26" s="164"/>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="248" t="s">
+      <c r="C27" s="250" t="s">
         <v>307</v>
       </c>
       <c r="D27" s="65" t="s">
@@ -12275,14 +12670,14 @@
       <c r="G27" s="68"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="249"/>
+      <c r="C28" s="251"/>
       <c r="D28" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C29" s="249"/>
+      <c r="C29" s="251"/>
       <c r="D29" s="56" t="s">
         <v>34</v>
       </c>
@@ -12295,7 +12690,7 @@
       <c r="G29" s="57"/>
     </row>
     <row r="30" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C30" s="249"/>
+      <c r="C30" s="251"/>
       <c r="D30" s="54" t="s">
         <v>113</v>
       </c>
@@ -12304,7 +12699,7 @@
       <c r="G30" s="57"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="249"/>
+      <c r="C31" s="251"/>
       <c r="D31" s="56" t="s">
         <v>114</v>
       </c>
@@ -12319,14 +12714,14 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="249"/>
+      <c r="C32" s="251"/>
       <c r="D32" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="249"/>
+      <c r="C33" s="251"/>
       <c r="D33" s="56" t="s">
         <v>98</v>
       </c>
@@ -12337,7 +12732,7 @@
       <c r="G33" s="55"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="249"/>
+      <c r="C34" s="251"/>
       <c r="D34" s="56" t="s">
         <v>97</v>
       </c>
@@ -12350,7 +12745,7 @@
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="249"/>
+      <c r="C35" s="251"/>
       <c r="D35" s="56" t="s">
         <v>102</v>
       </c>
@@ -12363,7 +12758,7 @@
       <c r="G35" s="55"/>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="249"/>
+      <c r="C36" s="251"/>
       <c r="D36" s="56" t="s">
         <v>103</v>
       </c>
@@ -12376,7 +12771,7 @@
       <c r="G36" s="55"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="249"/>
+      <c r="C37" s="251"/>
       <c r="D37" s="56" t="s">
         <v>94</v>
       </c>
@@ -12389,7 +12784,7 @@
       <c r="G37" s="55"/>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="249"/>
+      <c r="C38" s="251"/>
       <c r="D38" s="60" t="s">
         <v>95</v>
       </c>
@@ -12402,7 +12797,7 @@
       <c r="G38" s="63"/>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="249"/>
+      <c r="C39" s="251"/>
       <c r="D39" s="65" t="s">
         <v>116</v>
       </c>
@@ -12413,7 +12808,7 @@
       <c r="G39" s="68"/>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="249"/>
+      <c r="C40" s="251"/>
       <c r="D40" s="56" t="s">
         <v>119</v>
       </c>
@@ -12423,7 +12818,7 @@
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="249"/>
+      <c r="C41" s="251"/>
       <c r="D41" s="60" t="s">
         <v>121</v>
       </c>
@@ -12434,7 +12829,7 @@
       <c r="G41" s="63"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="249"/>
+      <c r="C42" s="251"/>
       <c r="D42" s="65" t="s">
         <v>116</v>
       </c>
@@ -12445,7 +12840,7 @@
       <c r="G42" s="68"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="249"/>
+      <c r="C43" s="251"/>
       <c r="D43" s="56" t="s">
         <v>126</v>
       </c>
@@ -12458,7 +12853,7 @@
       <c r="G43" s="55"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="249"/>
+      <c r="C44" s="251"/>
       <c r="D44" s="56" t="s">
         <v>119</v>
       </c>
@@ -12471,7 +12866,7 @@
       <c r="G44" s="55"/>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="250"/>
+      <c r="C45" s="252"/>
       <c r="D45" s="60" t="s">
         <v>110</v>
       </c>
@@ -12484,7 +12879,7 @@
       <c r="G45" s="63"/>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="248" t="s">
+      <c r="C46" s="250" t="s">
         <v>308</v>
       </c>
       <c r="D46" s="65" t="s">
@@ -12497,14 +12892,14 @@
       <c r="G46" s="68"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="249"/>
+      <c r="C47" s="251"/>
       <c r="D47" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G47" s="55"/>
     </row>
     <row r="48" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C48" s="249"/>
+      <c r="C48" s="251"/>
       <c r="D48" s="56" t="s">
         <v>34</v>
       </c>
@@ -12517,7 +12912,7 @@
       <c r="G48" s="57"/>
     </row>
     <row r="49" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C49" s="249"/>
+      <c r="C49" s="251"/>
       <c r="D49" s="54" t="s">
         <v>113</v>
       </c>
@@ -12526,7 +12921,7 @@
       <c r="G49" s="57"/>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="249"/>
+      <c r="C50" s="251"/>
       <c r="D50" s="56" t="s">
         <v>114</v>
       </c>
@@ -12541,14 +12936,14 @@
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="249"/>
+      <c r="C51" s="251"/>
       <c r="D51" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G51" s="55"/>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="249"/>
+      <c r="C52" s="251"/>
       <c r="D52" s="56" t="s">
         <v>98</v>
       </c>
@@ -12559,7 +12954,7 @@
       <c r="G52" s="55"/>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="249"/>
+      <c r="C53" s="251"/>
       <c r="D53" s="56" t="s">
         <v>97</v>
       </c>
@@ -12572,7 +12967,7 @@
       <c r="G53" s="55"/>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="249"/>
+      <c r="C54" s="251"/>
       <c r="D54" s="56" t="s">
         <v>102</v>
       </c>
@@ -12585,7 +12980,7 @@
       <c r="G54" s="55"/>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="249"/>
+      <c r="C55" s="251"/>
       <c r="D55" s="56" t="s">
         <v>103</v>
       </c>
@@ -12598,7 +12993,7 @@
       <c r="G55" s="55"/>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="249"/>
+      <c r="C56" s="251"/>
       <c r="D56" s="56" t="s">
         <v>94</v>
       </c>
@@ -12611,7 +13006,7 @@
       <c r="G56" s="55"/>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="249"/>
+      <c r="C57" s="251"/>
       <c r="D57" s="60" t="s">
         <v>95</v>
       </c>
@@ -12624,7 +13019,7 @@
       <c r="G57" s="63"/>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="249"/>
+      <c r="C58" s="251"/>
       <c r="D58" s="65" t="s">
         <v>116</v>
       </c>
@@ -12635,7 +13030,7 @@
       <c r="G58" s="68"/>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="249"/>
+      <c r="C59" s="251"/>
       <c r="D59" s="56" t="s">
         <v>119</v>
       </c>
@@ -12645,7 +13040,7 @@
       <c r="G59" s="55"/>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="249"/>
+      <c r="C60" s="251"/>
       <c r="D60" s="60" t="s">
         <v>121</v>
       </c>
@@ -12656,7 +13051,7 @@
       <c r="G60" s="63"/>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="249"/>
+      <c r="C61" s="251"/>
       <c r="D61" s="65" t="s">
         <v>116</v>
       </c>
@@ -12667,7 +13062,7 @@
       <c r="G61" s="68"/>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="249"/>
+      <c r="C62" s="251"/>
       <c r="D62" s="56" t="s">
         <v>126</v>
       </c>
@@ -12680,7 +13075,7 @@
       <c r="G62" s="55"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="249"/>
+      <c r="C63" s="251"/>
       <c r="D63" s="56" t="s">
         <v>119</v>
       </c>
@@ -12693,7 +13088,7 @@
       <c r="G63" s="55"/>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="250"/>
+      <c r="C64" s="252"/>
       <c r="D64" s="60" t="s">
         <v>110</v>
       </c>
@@ -12706,7 +13101,7 @@
       <c r="G64" s="63"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="248" t="s">
+      <c r="C65" s="250" t="s">
         <v>309</v>
       </c>
       <c r="D65" s="65" t="s">
@@ -12719,14 +13114,14 @@
       <c r="G65" s="68"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="249"/>
+      <c r="C66" s="251"/>
       <c r="D66" s="54" t="s">
         <v>111</v>
       </c>
       <c r="G66" s="55"/>
     </row>
     <row r="67" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C67" s="249"/>
+      <c r="C67" s="251"/>
       <c r="D67" s="56" t="s">
         <v>34</v>
       </c>
@@ -12739,7 +13134,7 @@
       <c r="G67" s="57"/>
     </row>
     <row r="68" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C68" s="249"/>
+      <c r="C68" s="251"/>
       <c r="D68" s="54" t="s">
         <v>113</v>
       </c>
@@ -12748,7 +13143,7 @@
       <c r="G68" s="57"/>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="249"/>
+      <c r="C69" s="251"/>
       <c r="D69" s="56" t="s">
         <v>114</v>
       </c>
@@ -12764,14 +13159,14 @@
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="249"/>
+      <c r="C70" s="251"/>
       <c r="D70" s="54" t="s">
         <v>112</v>
       </c>
       <c r="G70" s="55"/>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="249"/>
+      <c r="C71" s="251"/>
       <c r="D71" s="56" t="s">
         <v>98</v>
       </c>
@@ -12782,7 +13177,7 @@
       <c r="G71" s="55"/>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="249"/>
+      <c r="C72" s="251"/>
       <c r="D72" s="56" t="s">
         <v>97</v>
       </c>
@@ -12795,7 +13190,7 @@
       <c r="G72" s="55"/>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="249"/>
+      <c r="C73" s="251"/>
       <c r="D73" s="56" t="s">
         <v>102</v>
       </c>
@@ -12808,7 +13203,7 @@
       <c r="G73" s="55"/>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="249"/>
+      <c r="C74" s="251"/>
       <c r="D74" s="56" t="s">
         <v>103</v>
       </c>
@@ -12821,7 +13216,7 @@
       <c r="G74" s="55"/>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="249"/>
+      <c r="C75" s="251"/>
       <c r="D75" s="56" t="s">
         <v>94</v>
       </c>
@@ -12834,7 +13229,7 @@
       <c r="G75" s="55"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="249"/>
+      <c r="C76" s="251"/>
       <c r="D76" s="60" t="s">
         <v>95</v>
       </c>
@@ -12847,7 +13242,7 @@
       <c r="G76" s="63"/>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="249"/>
+      <c r="C77" s="251"/>
       <c r="D77" s="65" t="s">
         <v>116</v>
       </c>
@@ -12858,7 +13253,7 @@
       <c r="G77" s="68"/>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="249"/>
+      <c r="C78" s="251"/>
       <c r="D78" s="56" t="s">
         <v>119</v>
       </c>
@@ -12868,7 +13263,7 @@
       <c r="G78" s="55"/>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="249"/>
+      <c r="C79" s="251"/>
       <c r="D79" s="60" t="s">
         <v>121</v>
       </c>
@@ -12879,7 +13274,7 @@
       <c r="G79" s="63"/>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="249"/>
+      <c r="C80" s="251"/>
       <c r="D80" s="65" t="s">
         <v>116</v>
       </c>
@@ -12890,7 +13285,7 @@
       <c r="G80" s="68"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="249"/>
+      <c r="C81" s="251"/>
       <c r="D81" s="56" t="s">
         <v>126</v>
       </c>
@@ -12903,7 +13298,7 @@
       <c r="G81" s="55"/>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="249"/>
+      <c r="C82" s="251"/>
       <c r="D82" s="56" t="s">
         <v>119</v>
       </c>
@@ -12916,7 +13311,7 @@
       <c r="G82" s="55"/>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="250"/>
+      <c r="C83" s="252"/>
       <c r="D83" s="60" t="s">
         <v>110</v>
       </c>
@@ -13010,12 +13405,12 @@
       <c r="V8" s="75"/>
     </row>
     <row r="9" spans="4:23" x14ac:dyDescent="0.25">
-      <c r="D9" s="264" t="s">
+      <c r="D9" s="266" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="265"/>
-      <c r="F9" s="265"/>
-      <c r="G9" s="266"/>
+      <c r="E9" s="267"/>
+      <c r="F9" s="267"/>
+      <c r="G9" s="268"/>
       <c r="V9" s="75"/>
     </row>
     <row r="10" spans="4:23" x14ac:dyDescent="0.25">
@@ -13189,7 +13584,7 @@
       </c>
     </row>
     <row r="17" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D17" s="235" t="s">
+      <c r="D17" s="237" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="69" t="s">
@@ -13213,7 +13608,7 @@
       <c r="V17" s="75"/>
     </row>
     <row r="18" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D18" s="235"/>
+      <c r="D18" s="237"/>
       <c r="E18" s="69" t="s">
         <v>140</v>
       </c>
@@ -13235,7 +13630,7 @@
       <c r="V18" s="75"/>
     </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D19" s="235"/>
+      <c r="D19" s="237"/>
       <c r="E19" s="69" t="s">
         <v>141</v>
       </c>
@@ -13361,7 +13756,7 @@
       <c r="D31" s="96"/>
     </row>
     <row r="32" spans="3:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="267" t="s">
+      <c r="C32" s="269" t="s">
         <v>207</v>
       </c>
       <c r="D32" s="85" t="s">
@@ -13372,7 +13767,7 @@
       <c r="G32" s="87"/>
     </row>
     <row r="33" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C33" s="268"/>
+      <c r="C33" s="270"/>
       <c r="D33" s="89" t="s">
         <v>180</v>
       </c>
@@ -13383,7 +13778,7 @@
       <c r="G33" s="87"/>
     </row>
     <row r="34" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C34" s="268"/>
+      <c r="C34" s="270"/>
       <c r="D34" s="90" t="s">
         <v>181</v>
       </c>
@@ -13393,7 +13788,7 @@
       <c r="G34" s="88"/>
     </row>
     <row r="35" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C35" s="268"/>
+      <c r="C35" s="270"/>
       <c r="D35" s="90" t="s">
         <v>183</v>
       </c>
@@ -13405,7 +13800,7 @@
       </c>
     </row>
     <row r="36" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C36" s="268"/>
+      <c r="C36" s="270"/>
       <c r="D36" s="91" t="s">
         <v>185</v>
       </c>
@@ -13420,7 +13815,7 @@
       </c>
     </row>
     <row r="37" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C37" s="268"/>
+      <c r="C37" s="270"/>
       <c r="D37" s="94" t="s">
         <v>187</v>
       </c>
@@ -13433,7 +13828,7 @@
       </c>
     </row>
     <row r="38" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C38" s="268"/>
+      <c r="C38" s="270"/>
       <c r="D38" s="89" t="s">
         <v>193</v>
       </c>
@@ -13458,7 +13853,7 @@
       </c>
     </row>
     <row r="39" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C39" s="268"/>
+      <c r="C39" s="270"/>
       <c r="D39" s="90" t="s">
         <v>194</v>
       </c>
@@ -13480,7 +13875,7 @@
       </c>
     </row>
     <row r="40" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C40" s="268"/>
+      <c r="C40" s="270"/>
       <c r="D40" s="90" t="s">
         <v>195</v>
       </c>
@@ -13521,7 +13916,7 @@
       </c>
     </row>
     <row r="41" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C41" s="268"/>
+      <c r="C41" s="270"/>
       <c r="D41" s="91" t="s">
         <v>196</v>
       </c>
@@ -13562,7 +13957,7 @@
       </c>
     </row>
     <row r="42" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C42" s="268"/>
+      <c r="C42" s="270"/>
       <c r="D42" s="80" t="s">
         <v>197</v>
       </c>
@@ -13595,15 +13990,15 @@
       </c>
     </row>
     <row r="43" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C43" s="268"/>
+      <c r="C43" s="270"/>
       <c r="D43" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E43" s="259" t="s">
+      <c r="E43" s="261" t="s">
         <v>200</v>
       </c>
-      <c r="F43" s="259"/>
-      <c r="G43" s="260"/>
+      <c r="F43" s="261"/>
+      <c r="G43" s="262"/>
       <c r="AA43" s="44">
         <v>13</v>
       </c>
@@ -13632,13 +14027,13 @@
       </c>
     </row>
     <row r="44" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C44" s="269"/>
+      <c r="C44" s="271"/>
       <c r="D44" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="E44" s="261"/>
-      <c r="F44" s="261"/>
-      <c r="G44" s="262"/>
+      <c r="E44" s="263"/>
+      <c r="F44" s="263"/>
+      <c r="G44" s="264"/>
       <c r="AA44" s="44">
         <v>14</v>
       </c>
@@ -13667,7 +14062,7 @@
       </c>
     </row>
     <row r="45" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C45" s="263" t="s">
+      <c r="C45" s="265" t="s">
         <v>216</v>
       </c>
       <c r="D45" s="94" t="s">
@@ -13704,7 +14099,7 @@
       </c>
     </row>
     <row r="46" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C46" s="263"/>
+      <c r="C46" s="265"/>
       <c r="D46" s="89" t="s">
         <v>180</v>
       </c>
@@ -13741,7 +14136,7 @@
       </c>
     </row>
     <row r="47" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C47" s="263"/>
+      <c r="C47" s="265"/>
       <c r="D47" s="90" t="s">
         <v>181</v>
       </c>
@@ -13777,7 +14172,7 @@
       </c>
     </row>
     <row r="48" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C48" s="263"/>
+      <c r="C48" s="265"/>
       <c r="D48" s="90" t="s">
         <v>183</v>
       </c>
@@ -13815,7 +14210,7 @@
       </c>
     </row>
     <row r="49" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C49" s="263"/>
+      <c r="C49" s="265"/>
       <c r="D49" s="90" t="s">
         <v>185</v>
       </c>
@@ -13856,7 +14251,7 @@
       </c>
     </row>
     <row r="50" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C50" s="263"/>
+      <c r="C50" s="265"/>
       <c r="D50" s="93" t="s">
         <v>187</v>
       </c>
@@ -13889,7 +14284,7 @@
       </c>
     </row>
     <row r="51" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C51" s="263"/>
+      <c r="C51" s="265"/>
       <c r="D51" s="90" t="s">
         <v>212</v>
       </c>
@@ -13930,7 +14325,7 @@
       </c>
     </row>
     <row r="52" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C52" s="263"/>
+      <c r="C52" s="265"/>
       <c r="D52" s="93" t="s">
         <v>197</v>
       </c>
@@ -13963,15 +14358,15 @@
       </c>
     </row>
     <row r="53" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C53" s="263"/>
+      <c r="C53" s="265"/>
       <c r="D53" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="259" t="s">
+      <c r="E53" s="261" t="s">
         <v>200</v>
       </c>
-      <c r="F53" s="259"/>
-      <c r="G53" s="260"/>
+      <c r="F53" s="261"/>
+      <c r="G53" s="262"/>
       <c r="AA53" s="44">
         <v>23</v>
       </c>
@@ -14000,13 +14395,13 @@
       </c>
     </row>
     <row r="54" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C54" s="263"/>
+      <c r="C54" s="265"/>
       <c r="D54" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E54" s="261"/>
-      <c r="F54" s="261"/>
-      <c r="G54" s="262"/>
+      <c r="E54" s="263"/>
+      <c r="F54" s="263"/>
+      <c r="G54" s="264"/>
       <c r="AA54" s="44">
         <v>24</v>
       </c>
@@ -14035,7 +14430,7 @@
       </c>
     </row>
     <row r="55" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C55" s="263"/>
+      <c r="C55" s="265"/>
       <c r="D55" s="94" t="s">
         <v>186</v>
       </c>
@@ -14070,7 +14465,7 @@
       </c>
     </row>
     <row r="56" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C56" s="263"/>
+      <c r="C56" s="265"/>
       <c r="D56" s="89" t="s">
         <v>180</v>
       </c>
@@ -14107,7 +14502,7 @@
       </c>
     </row>
     <row r="57" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C57" s="263"/>
+      <c r="C57" s="265"/>
       <c r="D57" s="90" t="s">
         <v>181</v>
       </c>
@@ -14143,7 +14538,7 @@
       </c>
     </row>
     <row r="58" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C58" s="263"/>
+      <c r="C58" s="265"/>
       <c r="D58" s="90" t="s">
         <v>183</v>
       </c>
@@ -14181,7 +14576,7 @@
       </c>
     </row>
     <row r="59" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C59" s="263"/>
+      <c r="C59" s="265"/>
       <c r="D59" s="91" t="s">
         <v>185</v>
       </c>
@@ -14222,7 +14617,7 @@
       </c>
     </row>
     <row r="60" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C60" s="263"/>
+      <c r="C60" s="265"/>
       <c r="D60" s="94" t="s">
         <v>187</v>
       </c>
@@ -14257,7 +14652,7 @@
       </c>
     </row>
     <row r="61" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C61" s="263"/>
+      <c r="C61" s="265"/>
       <c r="D61" s="89" t="s">
         <v>212</v>
       </c>
@@ -14298,7 +14693,7 @@
       </c>
     </row>
     <row r="62" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C62" s="263"/>
+      <c r="C62" s="265"/>
       <c r="D62" s="93" t="s">
         <v>197</v>
       </c>
@@ -14331,15 +14726,15 @@
       </c>
     </row>
     <row r="63" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C63" s="263"/>
+      <c r="C63" s="265"/>
       <c r="D63" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="E63" s="259" t="s">
+      <c r="E63" s="261" t="s">
         <v>200</v>
       </c>
-      <c r="F63" s="259"/>
-      <c r="G63" s="260"/>
+      <c r="F63" s="261"/>
+      <c r="G63" s="262"/>
       <c r="AA63" s="44">
         <v>33</v>
       </c>
@@ -14368,13 +14763,13 @@
       </c>
     </row>
     <row r="64" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C64" s="263"/>
+      <c r="C64" s="265"/>
       <c r="D64" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="E64" s="261"/>
-      <c r="F64" s="261"/>
-      <c r="G64" s="262"/>
+      <c r="E64" s="263"/>
+      <c r="F64" s="263"/>
+      <c r="G64" s="264"/>
       <c r="AA64" s="44">
         <v>34</v>
       </c>
@@ -14526,22 +14921,22 @@
       </c>
     </row>
     <row r="69" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C69" s="267" t="s">
+      <c r="C69" s="269" t="s">
         <v>160</v>
       </c>
-      <c r="D69" s="273" t="s">
+      <c r="D69" s="275" t="s">
         <v>161</v>
       </c>
-      <c r="E69" s="273"/>
-      <c r="F69" s="273" t="s">
+      <c r="E69" s="275"/>
+      <c r="F69" s="275" t="s">
         <v>133</v>
       </c>
-      <c r="G69" s="274"/>
-      <c r="I69" s="270" t="s">
+      <c r="G69" s="276"/>
+      <c r="I69" s="272" t="s">
         <v>223</v>
       </c>
-      <c r="J69" s="271"/>
-      <c r="K69" s="272"/>
+      <c r="J69" s="273"/>
+      <c r="K69" s="274"/>
       <c r="AA69" s="44">
         <v>39</v>
       </c>
@@ -14570,7 +14965,7 @@
       </c>
     </row>
     <row r="70" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C70" s="268"/>
+      <c r="C70" s="270"/>
       <c r="D70" s="15" t="s">
         <v>162</v>
       </c>
@@ -14978,11 +15373,11 @@
         <f t="shared" si="10"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="I77" s="270" t="s">
+      <c r="I77" s="272" t="s">
         <v>222</v>
       </c>
-      <c r="J77" s="271"/>
-      <c r="K77" s="272"/>
+      <c r="J77" s="273"/>
+      <c r="K77" s="274"/>
       <c r="AA77" s="44">
         <v>47</v>
       </c>
@@ -15502,7 +15897,7 @@
       </c>
     </row>
     <row r="90" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C90" s="255" t="s">
+      <c r="C90" s="257" t="s">
         <v>230</v>
       </c>
       <c r="D90" s="86" t="s">
@@ -15555,7 +15950,7 @@
       </c>
     </row>
     <row r="91" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C91" s="256"/>
+      <c r="C91" s="258"/>
       <c r="D91" s="44" t="s">
         <v>232</v>
       </c>
@@ -15606,7 +16001,7 @@
       </c>
     </row>
     <row r="92" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C92" s="256" t="s">
+      <c r="C92" s="258" t="s">
         <v>233</v>
       </c>
       <c r="D92" s="44" t="s">
@@ -15659,7 +16054,7 @@
       </c>
     </row>
     <row r="93" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C93" s="256"/>
+      <c r="C93" s="258"/>
       <c r="D93" s="44" t="s">
         <v>236</v>
       </c>
@@ -15710,7 +16105,7 @@
       </c>
     </row>
     <row r="94" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C94" s="257" t="s">
+      <c r="C94" s="259" t="s">
         <v>234</v>
       </c>
       <c r="D94" s="44" t="s">
@@ -15763,7 +16158,7 @@
       </c>
     </row>
     <row r="95" spans="3:37" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C95" s="258"/>
+      <c r="C95" s="260"/>
       <c r="D95" s="81" t="s">
         <v>238</v>
       </c>
@@ -16131,7 +16526,7 @@
       </c>
     </row>
     <row r="126" spans="3:24" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C126" s="255" t="s">
+      <c r="C126" s="257" t="s">
         <v>230</v>
       </c>
       <c r="D126" s="86" t="s">
@@ -16158,7 +16553,7 @@
       </c>
     </row>
     <row r="127" spans="3:24" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C127" s="256"/>
+      <c r="C127" s="258"/>
       <c r="D127" s="44" t="s">
         <v>232</v>
       </c>
@@ -16183,7 +16578,7 @@
       </c>
     </row>
     <row r="128" spans="3:24" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C128" s="256" t="s">
+      <c r="C128" s="258" t="s">
         <v>233</v>
       </c>
       <c r="D128" s="44" t="s">
@@ -16210,7 +16605,7 @@
       </c>
     </row>
     <row r="129" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C129" s="256"/>
+      <c r="C129" s="258"/>
       <c r="D129" s="44" t="s">
         <v>236</v>
       </c>
@@ -16235,7 +16630,7 @@
       </c>
     </row>
     <row r="130" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C130" s="257" t="s">
+      <c r="C130" s="259" t="s">
         <v>234</v>
       </c>
       <c r="D130" s="44" t="s">
@@ -16262,7 +16657,7 @@
       </c>
     </row>
     <row r="131" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C131" s="258"/>
+      <c r="C131" s="260"/>
       <c r="D131" s="81" t="s">
         <v>238</v>
       </c>
@@ -16497,7 +16892,7 @@
       </c>
     </row>
     <row r="163" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C163" s="255" t="s">
+      <c r="C163" s="257" t="s">
         <v>230</v>
       </c>
       <c r="D163" s="86" t="s">
@@ -16524,7 +16919,7 @@
       </c>
     </row>
     <row r="164" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C164" s="256"/>
+      <c r="C164" s="258"/>
       <c r="D164" s="44" t="s">
         <v>232</v>
       </c>
@@ -16549,7 +16944,7 @@
       </c>
     </row>
     <row r="165" spans="3:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C165" s="256" t="s">
+      <c r="C165" s="258" t="s">
         <v>233</v>
       </c>
       <c r="D165" s="44" t="s">
@@ -16576,7 +16971,7 @@
       </c>
     </row>
     <row r="166" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C166" s="256"/>
+      <c r="C166" s="258"/>
       <c r="D166" s="44" t="s">
         <v>236</v>
       </c>
@@ -16601,7 +16996,7 @@
       </c>
     </row>
     <row r="167" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C167" s="257" t="s">
+      <c r="C167" s="259" t="s">
         <v>234</v>
       </c>
       <c r="D167" s="44" t="s">
@@ -16628,7 +17023,7 @@
       </c>
     </row>
     <row r="168" spans="3:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C168" s="258"/>
+      <c r="C168" s="260"/>
       <c r="D168" s="81" t="s">
         <v>238</v>
       </c>
@@ -16882,27 +17277,27 @@
       <c r="L4" s="81"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="270" t="s">
+      <c r="C5" s="272" t="s">
         <v>314</v>
       </c>
-      <c r="D5" s="271"/>
-      <c r="E5" s="271"/>
-      <c r="F5" s="271"/>
-      <c r="G5" s="271"/>
-      <c r="H5" s="272"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
+      <c r="G5" s="273"/>
+      <c r="H5" s="274"/>
       <c r="I5" s="171" t="s">
         <v>315</v>
       </c>
-      <c r="J5" s="270" t="s">
+      <c r="J5" s="272" t="s">
         <v>316</v>
       </c>
-      <c r="K5" s="271"/>
-      <c r="L5" s="271"/>
-      <c r="M5" s="275" t="s">
+      <c r="K5" s="273"/>
+      <c r="L5" s="273"/>
+      <c r="M5" s="277" t="s">
         <v>322</v>
       </c>
-      <c r="N5" s="273"/>
-      <c r="O5" s="274"/>
+      <c r="N5" s="275"/>
+      <c r="O5" s="276"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="168" t="s">
@@ -17108,26 +17503,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="D2" s="276" t="s">
+      <c r="D2" s="278" t="s">
         <v>356</v>
       </c>
-      <c r="E2" s="277"/>
-      <c r="F2" s="277"/>
-      <c r="G2" s="277"/>
-      <c r="H2" s="277"/>
-      <c r="I2" s="277"/>
-      <c r="J2" s="277"/>
-      <c r="K2" s="278"/>
-      <c r="L2" s="276" t="s">
+      <c r="E2" s="279"/>
+      <c r="F2" s="279"/>
+      <c r="G2" s="279"/>
+      <c r="H2" s="279"/>
+      <c r="I2" s="279"/>
+      <c r="J2" s="279"/>
+      <c r="K2" s="280"/>
+      <c r="L2" s="278" t="s">
         <v>357</v>
       </c>
-      <c r="M2" s="277"/>
-      <c r="N2" s="277"/>
-      <c r="O2" s="277"/>
-      <c r="P2" s="277"/>
-      <c r="Q2" s="277"/>
-      <c r="R2" s="277"/>
-      <c r="S2" s="278"/>
+      <c r="M2" s="279"/>
+      <c r="N2" s="279"/>
+      <c r="O2" s="279"/>
+      <c r="P2" s="279"/>
+      <c r="Q2" s="279"/>
+      <c r="R2" s="279"/>
+      <c r="S2" s="280"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B3" s="204" t="s">
@@ -18089,14 +18484,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E5" s="279" t="s">
+      <c r="E5" s="281" t="s">
         <v>366</v>
       </c>
-      <c r="F5" s="280"/>
-      <c r="G5" s="281" t="s">
+      <c r="F5" s="282"/>
+      <c r="G5" s="283" t="s">
         <v>367</v>
       </c>
-      <c r="H5" s="282"/>
+      <c r="H5" s="284"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="217" t="s">

</xml_diff>